<commit_message>
Important check in to correct pin assignment and remove pull-down resistor
</commit_message>
<xml_diff>
--- a/Baseboard/BBmapping.xlsx
+++ b/Baseboard/BBmapping.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\project\wolf\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\work\wolf\Baseboard\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1560" uniqueCount="482">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1560" uniqueCount="484">
   <si>
     <t>LOCATE COMP "DRV0_PWROK" SITE "M4" ;</t>
   </si>
@@ -1477,6 +1477,14 @@
   </si>
   <si>
     <t>LOCATE COMP "DRV</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>_PWROK" SITE "Y1" ;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>_PCIE_CLK_A_OE_L" SITE "W6" ;</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -7502,9 +7510,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C216"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A194" workbookViewId="0">
-      <selection activeCell="C216" sqref="C216"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
@@ -7562,10 +7568,10 @@
         <v>264</v>
       </c>
       <c r="B5" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C5" t="s">
-        <v>386</v>
+        <v>483</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.15">
@@ -7573,10 +7579,10 @@
         <v>264</v>
       </c>
       <c r="B6" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C6" t="s">
-        <v>387</v>
+        <v>268</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.15">
@@ -7584,10 +7590,10 @@
         <v>264</v>
       </c>
       <c r="B7" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C7" t="s">
-        <v>388</v>
+        <v>271</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.15">
@@ -7598,7 +7604,7 @@
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.15">
@@ -7606,10 +7612,10 @@
         <v>264</v>
       </c>
       <c r="B9" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.15">
@@ -7617,10 +7623,10 @@
         <v>264</v>
       </c>
       <c r="B10" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.15">
@@ -7628,10 +7634,10 @@
         <v>264</v>
       </c>
       <c r="B11" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.15">
@@ -7639,10 +7645,10 @@
         <v>264</v>
       </c>
       <c r="B12" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>393</v>
+        <v>274</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.15">
@@ -7650,10 +7656,10 @@
         <v>264</v>
       </c>
       <c r="B13" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>394</v>
+        <v>275</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.15">
@@ -7661,10 +7667,10 @@
         <v>264</v>
       </c>
       <c r="B14" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C14" t="s">
-        <v>395</v>
+        <v>278</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.15">
@@ -7672,10 +7678,10 @@
         <v>264</v>
       </c>
       <c r="B15" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>396</v>
+        <v>390</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.15">
@@ -7683,10 +7689,10 @@
         <v>264</v>
       </c>
       <c r="B16" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C16" t="s">
-        <v>397</v>
+        <v>391</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.15">
@@ -7694,10 +7700,10 @@
         <v>264</v>
       </c>
       <c r="B17" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C17" t="s">
-        <v>398</v>
+        <v>392</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.15">
@@ -7705,10 +7711,10 @@
         <v>264</v>
       </c>
       <c r="B18" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C18" t="s">
-        <v>399</v>
+        <v>393</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.15">
@@ -7716,10 +7722,10 @@
         <v>264</v>
       </c>
       <c r="B19" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C19" t="s">
-        <v>400</v>
+        <v>351</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.15">
@@ -7727,10 +7733,10 @@
         <v>264</v>
       </c>
       <c r="B20" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C20" t="s">
-        <v>401</v>
+        <v>352</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.15">
@@ -7738,10 +7744,10 @@
         <v>264</v>
       </c>
       <c r="B21" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C21" t="s">
-        <v>402</v>
+        <v>355</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.15">
@@ -7749,10 +7755,10 @@
         <v>264</v>
       </c>
       <c r="B22" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C22" t="s">
-        <v>403</v>
+        <v>394</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.15">
@@ -7760,10 +7766,10 @@
         <v>264</v>
       </c>
       <c r="B23" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C23" t="s">
-        <v>404</v>
+        <v>395</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.15">
@@ -7771,10 +7777,10 @@
         <v>264</v>
       </c>
       <c r="B24" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C24" t="s">
-        <v>405</v>
+        <v>396</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.15">
@@ -7782,10 +7788,10 @@
         <v>264</v>
       </c>
       <c r="B25" s="1">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C25" t="s">
-        <v>413</v>
+        <v>397</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.15">
@@ -7793,10 +7799,10 @@
         <v>264</v>
       </c>
       <c r="B26" s="1">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C26" t="s">
-        <v>414</v>
+        <v>408</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.15">
@@ -7804,10 +7810,10 @@
         <v>264</v>
       </c>
       <c r="B27" s="1">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C27" t="s">
-        <v>415</v>
+        <v>409</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.15">
@@ -7815,10 +7821,10 @@
         <v>264</v>
       </c>
       <c r="B28" s="1">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C28" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.15">
@@ -7826,10 +7832,10 @@
         <v>264</v>
       </c>
       <c r="B29" s="1">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C29" t="s">
-        <v>417</v>
+        <v>398</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.15">
@@ -7837,10 +7843,10 @@
         <v>264</v>
       </c>
       <c r="B30" s="1">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C30" t="s">
-        <v>418</v>
+        <v>399</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.15">
@@ -7848,10 +7854,10 @@
         <v>264</v>
       </c>
       <c r="B31" s="1">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C31" t="s">
-        <v>419</v>
+        <v>400</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.15">
@@ -7859,10 +7865,10 @@
         <v>264</v>
       </c>
       <c r="B32" s="1">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C32" t="s">
-        <v>420</v>
+        <v>401</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.15">
@@ -7870,10 +7876,10 @@
         <v>264</v>
       </c>
       <c r="B33" s="1">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C33" t="s">
-        <v>421</v>
+        <v>439</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.15">
@@ -7881,10 +7887,10 @@
         <v>264</v>
       </c>
       <c r="B34" s="1">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C34" t="s">
-        <v>422</v>
+        <v>440</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.15">
@@ -7892,10 +7898,10 @@
         <v>264</v>
       </c>
       <c r="B35" s="1">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C35" t="s">
-        <v>423</v>
+        <v>443</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.15">
@@ -7903,10 +7909,10 @@
         <v>264</v>
       </c>
       <c r="B36" s="1">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C36" t="s">
-        <v>424</v>
+        <v>402</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.15">
@@ -7914,10 +7920,10 @@
         <v>264</v>
       </c>
       <c r="B37" s="1">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C37" t="s">
-        <v>425</v>
+        <v>403</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.15">
@@ -7925,10 +7931,10 @@
         <v>264</v>
       </c>
       <c r="B38" s="1">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C38" t="s">
-        <v>426</v>
+        <v>404</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.15">
@@ -7936,10 +7942,10 @@
         <v>264</v>
       </c>
       <c r="B39" s="1">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C39" t="s">
-        <v>427</v>
+        <v>405</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.15">
@@ -7947,10 +7953,10 @@
         <v>264</v>
       </c>
       <c r="B40" s="1">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C40" t="s">
-        <v>428</v>
+        <v>446</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.15">
@@ -7958,10 +7964,10 @@
         <v>264</v>
       </c>
       <c r="B41" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C41" t="s">
-        <v>429</v>
+        <v>447</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.15">
@@ -7969,10 +7975,10 @@
         <v>264</v>
       </c>
       <c r="B42" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C42" t="s">
-        <v>430</v>
+        <v>450</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.15">
@@ -7980,10 +7986,10 @@
         <v>264</v>
       </c>
       <c r="B43" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C43" t="s">
-        <v>431</v>
+        <v>413</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.15">
@@ -7991,10 +7997,10 @@
         <v>264</v>
       </c>
       <c r="B44" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C44" t="s">
-        <v>432</v>
+        <v>414</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.15">
@@ -8002,10 +8008,10 @@
         <v>264</v>
       </c>
       <c r="B45" s="1">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C45" t="s">
-        <v>433</v>
+        <v>415</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.15">
@@ -8013,10 +8019,10 @@
         <v>264</v>
       </c>
       <c r="B46" s="1">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C46" t="s">
-        <v>434</v>
+        <v>416</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.15">
@@ -8024,10 +8030,10 @@
         <v>264</v>
       </c>
       <c r="B47" s="1">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C47" t="s">
-        <v>435</v>
+        <v>453</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.15">
@@ -8035,10 +8041,10 @@
         <v>264</v>
       </c>
       <c r="B48" s="1">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C48" t="s">
-        <v>436</v>
+        <v>454</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.15">
@@ -8046,10 +8052,10 @@
         <v>264</v>
       </c>
       <c r="B49" s="1">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C49" t="s">
-        <v>293</v>
+        <v>457</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.15">
@@ -8057,10 +8063,10 @@
         <v>264</v>
       </c>
       <c r="B50" s="1">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C50" t="s">
-        <v>294</v>
+        <v>417</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.15">
@@ -8068,10 +8074,10 @@
         <v>264</v>
       </c>
       <c r="B51" s="1">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C51" t="s">
-        <v>295</v>
+        <v>418</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.15">
@@ -8079,10 +8085,10 @@
         <v>264</v>
       </c>
       <c r="B52" s="1">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C52" t="s">
-        <v>296</v>
+        <v>419</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.15">
@@ -8090,10 +8096,10 @@
         <v>264</v>
       </c>
       <c r="B53" s="1">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C53" t="s">
-        <v>297</v>
+        <v>420</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.15">
@@ -8101,10 +8107,10 @@
         <v>264</v>
       </c>
       <c r="B54" s="1">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C54" t="s">
-        <v>298</v>
+        <v>460</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.15">
@@ -8112,10 +8118,10 @@
         <v>264</v>
       </c>
       <c r="B55" s="1">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C55" t="s">
-        <v>299</v>
+        <v>461</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.15">
@@ -8123,10 +8129,10 @@
         <v>264</v>
       </c>
       <c r="B56" s="1">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C56" t="s">
-        <v>300</v>
+        <v>464</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.15">
@@ -8134,10 +8140,10 @@
         <v>264</v>
       </c>
       <c r="B57" s="1">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C57" t="s">
-        <v>301</v>
+        <v>421</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.15">
@@ -8145,10 +8151,10 @@
         <v>264</v>
       </c>
       <c r="B58" s="1">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C58" t="s">
-        <v>302</v>
+        <v>422</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.15">
@@ -8156,10 +8162,10 @@
         <v>264</v>
       </c>
       <c r="B59" s="1">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C59" t="s">
-        <v>303</v>
+        <v>423</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.15">
@@ -8167,10 +8173,10 @@
         <v>264</v>
       </c>
       <c r="B60" s="1">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C60" t="s">
-        <v>304</v>
+        <v>424</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.15">
@@ -8178,10 +8184,10 @@
         <v>264</v>
       </c>
       <c r="B61" s="1">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C61" t="s">
-        <v>305</v>
+        <v>467</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.15">
@@ -8189,10 +8195,10 @@
         <v>264</v>
       </c>
       <c r="B62" s="1">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C62" t="s">
-        <v>306</v>
+        <v>468</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.15">
@@ -8200,10 +8206,10 @@
         <v>264</v>
       </c>
       <c r="B63" s="1">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C63" t="s">
-        <v>307</v>
+        <v>471</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.15">
@@ -8211,10 +8217,10 @@
         <v>264</v>
       </c>
       <c r="B64" s="1">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C64" t="s">
-        <v>308</v>
+        <v>425</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.15">
@@ -8222,10 +8228,10 @@
         <v>264</v>
       </c>
       <c r="B65" s="1">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C65" t="s">
-        <v>309</v>
+        <v>426</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.15">
@@ -8233,10 +8239,10 @@
         <v>264</v>
       </c>
       <c r="B66" s="1">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C66" t="s">
-        <v>310</v>
+        <v>427</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.15">
@@ -8244,10 +8250,10 @@
         <v>264</v>
       </c>
       <c r="B67" s="1">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C67" t="s">
-        <v>311</v>
+        <v>428</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.15">
@@ -8255,10 +8261,10 @@
         <v>264</v>
       </c>
       <c r="B68" s="1">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C68" t="s">
-        <v>312</v>
+        <v>474</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.15">
@@ -8266,10 +8272,10 @@
         <v>264</v>
       </c>
       <c r="B69" s="1">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C69" t="s">
-        <v>313</v>
+        <v>475</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.15">
@@ -8277,10 +8283,10 @@
         <v>264</v>
       </c>
       <c r="B70" s="1">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="C70" t="s">
-        <v>314</v>
+        <v>478</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.15">
@@ -8288,10 +8294,10 @@
         <v>264</v>
       </c>
       <c r="B71" s="1">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C71" t="s">
-        <v>315</v>
+        <v>429</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.15">
@@ -8299,10 +8305,10 @@
         <v>264</v>
       </c>
       <c r="B72" s="1">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C72" t="s">
-        <v>316</v>
+        <v>430</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.15">
@@ -8310,10 +8316,10 @@
         <v>264</v>
       </c>
       <c r="B73" s="1">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C73" t="s">
-        <v>317</v>
+        <v>431</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.15">
@@ -8321,10 +8327,10 @@
         <v>264</v>
       </c>
       <c r="B74" s="1">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C74" t="s">
-        <v>318</v>
+        <v>432</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.15">
@@ -8332,10 +8338,10 @@
         <v>264</v>
       </c>
       <c r="B75" s="1">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C75" t="s">
-        <v>319</v>
+        <v>281</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.15">
@@ -8343,10 +8349,10 @@
         <v>264</v>
       </c>
       <c r="B76" s="1">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C76" t="s">
-        <v>320</v>
+        <v>282</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.15">
@@ -8354,10 +8360,10 @@
         <v>264</v>
       </c>
       <c r="B77" s="1">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C77" t="s">
-        <v>321</v>
+        <v>285</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.15">
@@ -8365,10 +8371,10 @@
         <v>264</v>
       </c>
       <c r="B78" s="1">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C78" t="s">
-        <v>322</v>
+        <v>433</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.15">
@@ -8376,10 +8382,10 @@
         <v>264</v>
       </c>
       <c r="B79" s="1">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C79" t="s">
-        <v>323</v>
+        <v>434</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.15">
@@ -8387,10 +8393,10 @@
         <v>264</v>
       </c>
       <c r="B80" s="1">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C80" t="s">
-        <v>324</v>
+        <v>435</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.15">
@@ -8398,10 +8404,10 @@
         <v>264</v>
       </c>
       <c r="B81" s="1">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C81" t="s">
-        <v>325</v>
+        <v>436</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.15">
@@ -8409,10 +8415,10 @@
         <v>264</v>
       </c>
       <c r="B82" s="1">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C82" t="s">
-        <v>326</v>
+        <v>288</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.15">
@@ -8420,10 +8426,10 @@
         <v>264</v>
       </c>
       <c r="B83" s="1">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C83" t="s">
-        <v>327</v>
+        <v>289</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.15">
@@ -8431,10 +8437,10 @@
         <v>264</v>
       </c>
       <c r="B84" s="1">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="C84" t="s">
-        <v>328</v>
+        <v>482</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.15">
@@ -8442,10 +8448,10 @@
         <v>264</v>
       </c>
       <c r="B85" s="1">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C85" t="s">
-        <v>329</v>
+        <v>293</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.15">
@@ -8453,10 +8459,10 @@
         <v>264</v>
       </c>
       <c r="B86" s="1">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C86" t="s">
-        <v>330</v>
+        <v>294</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.15">
@@ -8464,10 +8470,10 @@
         <v>264</v>
       </c>
       <c r="B87" s="1">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C87" t="s">
-        <v>331</v>
+        <v>295</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.15">
@@ -8475,10 +8481,10 @@
         <v>264</v>
       </c>
       <c r="B88" s="1">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C88" t="s">
-        <v>332</v>
+        <v>296</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.15">
@@ -8486,10 +8492,10 @@
         <v>264</v>
       </c>
       <c r="B89" s="1">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C89" t="s">
-        <v>333</v>
+        <v>297</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.15">
@@ -8497,10 +8503,10 @@
         <v>264</v>
       </c>
       <c r="B90" s="1">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C90" t="s">
-        <v>334</v>
+        <v>298</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.15">
@@ -8508,10 +8514,10 @@
         <v>264</v>
       </c>
       <c r="B91" s="1">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C91" t="s">
-        <v>335</v>
+        <v>299</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.15">
@@ -8519,10 +8525,10 @@
         <v>264</v>
       </c>
       <c r="B92" s="1">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C92" t="s">
-        <v>336</v>
+        <v>300</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.15">
@@ -8530,10 +8536,10 @@
         <v>264</v>
       </c>
       <c r="B93" s="1">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C93" t="s">
-        <v>337</v>
+        <v>301</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.15">
@@ -8541,10 +8547,10 @@
         <v>264</v>
       </c>
       <c r="B94" s="1">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C94" t="s">
-        <v>338</v>
+        <v>302</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.15">
@@ -8552,10 +8558,10 @@
         <v>264</v>
       </c>
       <c r="B95" s="1">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C95" t="s">
-        <v>339</v>
+        <v>303</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.15">
@@ -8563,10 +8569,10 @@
         <v>264</v>
       </c>
       <c r="B96" s="1">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C96" t="s">
-        <v>340</v>
+        <v>304</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.15">
@@ -8574,10 +8580,10 @@
         <v>264</v>
       </c>
       <c r="B97" s="1">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C97" t="s">
-        <v>341</v>
+        <v>305</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.15">
@@ -8585,10 +8591,10 @@
         <v>264</v>
       </c>
       <c r="B98" s="1">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C98" t="s">
-        <v>342</v>
+        <v>306</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.15">
@@ -8596,10 +8602,10 @@
         <v>264</v>
       </c>
       <c r="B99" s="1">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C99" t="s">
-        <v>343</v>
+        <v>307</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.15">
@@ -8607,10 +8613,10 @@
         <v>264</v>
       </c>
       <c r="B100" s="1">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C100" t="s">
-        <v>344</v>
+        <v>308</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.15">
@@ -8618,10 +8624,10 @@
         <v>264</v>
       </c>
       <c r="B101" s="1">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C101" t="s">
-        <v>345</v>
+        <v>309</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.15">
@@ -8629,10 +8635,10 @@
         <v>264</v>
       </c>
       <c r="B102" s="1">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C102" t="s">
-        <v>346</v>
+        <v>310</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.15">
@@ -8640,10 +8646,10 @@
         <v>264</v>
       </c>
       <c r="B103" s="1">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C103" t="s">
-        <v>347</v>
+        <v>311</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.15">
@@ -8651,10 +8657,10 @@
         <v>264</v>
       </c>
       <c r="B104" s="1">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C104" t="s">
-        <v>348</v>
+        <v>312</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.15">
@@ -8662,10 +8668,10 @@
         <v>264</v>
       </c>
       <c r="B105" s="1">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C105" t="s">
-        <v>356</v>
+        <v>313</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.15">
@@ -8673,10 +8679,10 @@
         <v>264</v>
       </c>
       <c r="B106" s="1">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C106" t="s">
-        <v>357</v>
+        <v>314</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.15">
@@ -8684,10 +8690,10 @@
         <v>264</v>
       </c>
       <c r="B107" s="1">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C107" t="s">
-        <v>358</v>
+        <v>315</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.15">
@@ -8695,10 +8701,10 @@
         <v>264</v>
       </c>
       <c r="B108" s="1">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C108" t="s">
-        <v>359</v>
+        <v>316</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.15">
@@ -8706,10 +8712,10 @@
         <v>264</v>
       </c>
       <c r="B109" s="1">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C109" t="s">
-        <v>360</v>
+        <v>317</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.15">
@@ -8717,10 +8723,10 @@
         <v>264</v>
       </c>
       <c r="B110" s="1">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C110" t="s">
-        <v>361</v>
+        <v>318</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.15">
@@ -8728,10 +8734,10 @@
         <v>264</v>
       </c>
       <c r="B111" s="1">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C111" t="s">
-        <v>362</v>
+        <v>319</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.15">
@@ -8739,10 +8745,10 @@
         <v>264</v>
       </c>
       <c r="B112" s="1">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C112" t="s">
-        <v>363</v>
+        <v>320</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.15">
@@ -8750,10 +8756,10 @@
         <v>264</v>
       </c>
       <c r="B113" s="1">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C113" t="s">
-        <v>364</v>
+        <v>321</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.15">
@@ -8761,10 +8767,10 @@
         <v>264</v>
       </c>
       <c r="B114" s="1">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C114" t="s">
-        <v>365</v>
+        <v>322</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.15">
@@ -8772,10 +8778,10 @@
         <v>264</v>
       </c>
       <c r="B115" s="1">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C115" t="s">
-        <v>366</v>
+        <v>323</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.15">
@@ -8783,10 +8789,10 @@
         <v>264</v>
       </c>
       <c r="B116" s="1">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C116" t="s">
-        <v>367</v>
+        <v>324</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.15">
@@ -8794,10 +8800,10 @@
         <v>264</v>
       </c>
       <c r="B117" s="1">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C117" t="s">
-        <v>368</v>
+        <v>325</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.15">
@@ -8805,10 +8811,10 @@
         <v>264</v>
       </c>
       <c r="B118" s="1">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C118" t="s">
-        <v>369</v>
+        <v>326</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.15">
@@ -8816,10 +8822,10 @@
         <v>264</v>
       </c>
       <c r="B119" s="1">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C119" t="s">
-        <v>370</v>
+        <v>327</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.15">
@@ -8827,10 +8833,10 @@
         <v>264</v>
       </c>
       <c r="B120" s="1">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C120" t="s">
-        <v>371</v>
+        <v>328</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.15">
@@ -8838,10 +8844,10 @@
         <v>264</v>
       </c>
       <c r="B121" s="1">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C121" t="s">
-        <v>372</v>
+        <v>329</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.15">
@@ -8849,10 +8855,10 @@
         <v>264</v>
       </c>
       <c r="B122" s="1">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C122" t="s">
-        <v>373</v>
+        <v>330</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.15">
@@ -8860,10 +8866,10 @@
         <v>264</v>
       </c>
       <c r="B123" s="1">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C123" t="s">
-        <v>374</v>
+        <v>331</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.15">
@@ -8871,10 +8877,10 @@
         <v>264</v>
       </c>
       <c r="B124" s="1">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C124" t="s">
-        <v>375</v>
+        <v>332</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.15">
@@ -8882,10 +8888,10 @@
         <v>264</v>
       </c>
       <c r="B125" s="1">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C125" t="s">
-        <v>376</v>
+        <v>333</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.15">
@@ -8893,10 +8899,10 @@
         <v>264</v>
       </c>
       <c r="B126" s="1">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C126" t="s">
-        <v>377</v>
+        <v>334</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.15">
@@ -8904,10 +8910,10 @@
         <v>264</v>
       </c>
       <c r="B127" s="1">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C127" t="s">
-        <v>378</v>
+        <v>335</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.15">
@@ -8915,10 +8921,10 @@
         <v>264</v>
       </c>
       <c r="B128" s="1">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C128" t="s">
-        <v>379</v>
+        <v>336</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.15">
@@ -8926,10 +8932,10 @@
         <v>264</v>
       </c>
       <c r="B129" s="1">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C129" t="s">
-        <v>380</v>
+        <v>337</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.15">
@@ -8937,10 +8943,10 @@
         <v>264</v>
       </c>
       <c r="B130" s="1">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C130" t="s">
-        <v>381</v>
+        <v>338</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.15">
@@ -8948,10 +8954,10 @@
         <v>264</v>
       </c>
       <c r="B131" s="1">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C131" t="s">
-        <v>382</v>
+        <v>339</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.15">
@@ -8959,21 +8965,21 @@
         <v>264</v>
       </c>
       <c r="B132" s="1">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C132" t="s">
-        <v>479</v>
+        <v>340</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A133" t="s">
-        <v>481</v>
+        <v>264</v>
       </c>
       <c r="B133" s="1">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C133" t="s">
-        <v>265</v>
+        <v>341</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.15">
@@ -8981,10 +8987,10 @@
         <v>264</v>
       </c>
       <c r="B134" s="1">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C134" t="s">
-        <v>266</v>
+        <v>342</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.15">
@@ -8992,10 +8998,10 @@
         <v>264</v>
       </c>
       <c r="B135" s="1">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C135" t="s">
-        <v>267</v>
+        <v>343</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.15">
@@ -9003,10 +9009,10 @@
         <v>264</v>
       </c>
       <c r="B136" s="1">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C136" t="s">
-        <v>268</v>
+        <v>344</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.15">
@@ -9014,10 +9020,10 @@
         <v>264</v>
       </c>
       <c r="B137" s="1">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C137" t="s">
-        <v>269</v>
+        <v>345</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.15">
@@ -9025,10 +9031,10 @@
         <v>264</v>
       </c>
       <c r="B138" s="1">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C138" t="s">
-        <v>270</v>
+        <v>346</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.15">
@@ -9036,10 +9042,10 @@
         <v>264</v>
       </c>
       <c r="B139" s="1">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C139" t="s">
-        <v>271</v>
+        <v>347</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.15">
@@ -9047,10 +9053,10 @@
         <v>264</v>
       </c>
       <c r="B140" s="1">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C140" t="s">
-        <v>272</v>
+        <v>348</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.15">
@@ -9058,10 +9064,10 @@
         <v>264</v>
       </c>
       <c r="B141" s="1">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C141" t="s">
-        <v>273</v>
+        <v>356</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.15">
@@ -9069,10 +9075,10 @@
         <v>264</v>
       </c>
       <c r="B142" s="1">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C142" t="s">
-        <v>274</v>
+        <v>357</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.15">
@@ -9080,10 +9086,10 @@
         <v>264</v>
       </c>
       <c r="B143" s="1">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C143" t="s">
-        <v>275</v>
+        <v>358</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.15">
@@ -9091,10 +9097,10 @@
         <v>264</v>
       </c>
       <c r="B144" s="1">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C144" t="s">
-        <v>276</v>
+        <v>359</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.15">
@@ -9102,10 +9108,10 @@
         <v>264</v>
       </c>
       <c r="B145" s="1">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C145" t="s">
-        <v>277</v>
+        <v>360</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.15">
@@ -9113,10 +9119,10 @@
         <v>264</v>
       </c>
       <c r="B146" s="1">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C146" t="s">
-        <v>278</v>
+        <v>361</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.15">
@@ -9124,10 +9130,10 @@
         <v>264</v>
       </c>
       <c r="B147" s="1">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="C147" t="s">
-        <v>349</v>
+        <v>362</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.15">
@@ -9135,10 +9141,10 @@
         <v>264</v>
       </c>
       <c r="B148" s="1">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C148" t="s">
-        <v>350</v>
+        <v>363</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.15">
@@ -9146,10 +9152,10 @@
         <v>264</v>
       </c>
       <c r="B149" s="1">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C149" t="s">
-        <v>351</v>
+        <v>364</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.15">
@@ -9157,10 +9163,10 @@
         <v>264</v>
       </c>
       <c r="B150" s="1">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C150" t="s">
-        <v>352</v>
+        <v>365</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.15">
@@ -9168,10 +9174,10 @@
         <v>264</v>
       </c>
       <c r="B151" s="1">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C151" t="s">
-        <v>353</v>
+        <v>366</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.15">
@@ -9179,10 +9185,10 @@
         <v>264</v>
       </c>
       <c r="B152" s="1">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C152" t="s">
-        <v>354</v>
+        <v>367</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.15">
@@ -9190,10 +9196,10 @@
         <v>264</v>
       </c>
       <c r="B153" s="1">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C153" t="s">
-        <v>355</v>
+        <v>368</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.15">
@@ -9201,10 +9207,10 @@
         <v>264</v>
       </c>
       <c r="B154" s="1">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C154" t="s">
-        <v>406</v>
+        <v>369</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.15">
@@ -9212,10 +9218,10 @@
         <v>264</v>
       </c>
       <c r="B155" s="1">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C155" t="s">
-        <v>407</v>
+        <v>370</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.15">
@@ -9223,10 +9229,10 @@
         <v>264</v>
       </c>
       <c r="B156" s="1">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C156" t="s">
-        <v>408</v>
+        <v>371</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.15">
@@ -9234,10 +9240,10 @@
         <v>264</v>
       </c>
       <c r="B157" s="1">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C157" t="s">
-        <v>409</v>
+        <v>372</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.15">
@@ -9245,10 +9251,10 @@
         <v>264</v>
       </c>
       <c r="B158" s="1">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C158" t="s">
-        <v>410</v>
+        <v>373</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.15">
@@ -9256,10 +9262,10 @@
         <v>264</v>
       </c>
       <c r="B159" s="1">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C159" t="s">
-        <v>411</v>
+        <v>374</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.15">
@@ -9267,10 +9273,10 @@
         <v>264</v>
       </c>
       <c r="B160" s="1">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C160" t="s">
-        <v>412</v>
+        <v>375</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.15">
@@ -9278,10 +9284,10 @@
         <v>264</v>
       </c>
       <c r="B161" s="1">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="C161" t="s">
-        <v>437</v>
+        <v>376</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.15">
@@ -9289,10 +9295,10 @@
         <v>264</v>
       </c>
       <c r="B162" s="1">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C162" t="s">
-        <v>438</v>
+        <v>377</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.15">
@@ -9300,10 +9306,10 @@
         <v>264</v>
       </c>
       <c r="B163" s="1">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C163" t="s">
-        <v>439</v>
+        <v>378</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.15">
@@ -9311,10 +9317,10 @@
         <v>264</v>
       </c>
       <c r="B164" s="1">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C164" t="s">
-        <v>440</v>
+        <v>379</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.15">
@@ -9322,10 +9328,10 @@
         <v>264</v>
       </c>
       <c r="B165" s="1">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C165" t="s">
-        <v>441</v>
+        <v>380</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.15">
@@ -9333,10 +9339,10 @@
         <v>264</v>
       </c>
       <c r="B166" s="1">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C166" t="s">
-        <v>442</v>
+        <v>381</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.15">
@@ -9344,10 +9350,10 @@
         <v>264</v>
       </c>
       <c r="B167" s="1">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C167" t="s">
-        <v>443</v>
+        <v>382</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.15">
@@ -9355,21 +9361,21 @@
         <v>264</v>
       </c>
       <c r="B168" s="1">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="C168" t="s">
-        <v>444</v>
+        <v>479</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A169" t="s">
-        <v>264</v>
+        <v>481</v>
       </c>
       <c r="B169" s="1">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C169" t="s">
-        <v>445</v>
+        <v>265</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.15">
@@ -9377,10 +9383,10 @@
         <v>264</v>
       </c>
       <c r="B170" s="1">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C170" t="s">
-        <v>446</v>
+        <v>266</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.15">
@@ -9388,10 +9394,10 @@
         <v>264</v>
       </c>
       <c r="B171" s="1">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C171" t="s">
-        <v>447</v>
+        <v>269</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.15">
@@ -9399,10 +9405,10 @@
         <v>264</v>
       </c>
       <c r="B172" s="1">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C172" t="s">
-        <v>448</v>
+        <v>270</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.15">
@@ -9410,10 +9416,10 @@
         <v>264</v>
       </c>
       <c r="B173" s="1">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C173" t="s">
-        <v>449</v>
+        <v>272</v>
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.15">
@@ -9421,10 +9427,10 @@
         <v>264</v>
       </c>
       <c r="B174" s="1">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C174" t="s">
-        <v>450</v>
+        <v>273</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.15">
@@ -9432,10 +9438,10 @@
         <v>264</v>
       </c>
       <c r="B175" s="1">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C175" t="s">
-        <v>451</v>
+        <v>276</v>
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.15">
@@ -9443,10 +9449,10 @@
         <v>264</v>
       </c>
       <c r="B176" s="1">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C176" t="s">
-        <v>452</v>
+        <v>277</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.15">
@@ -9454,10 +9460,10 @@
         <v>264</v>
       </c>
       <c r="B177" s="1">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C177" t="s">
-        <v>453</v>
+        <v>349</v>
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.15">
@@ -9465,10 +9471,10 @@
         <v>264</v>
       </c>
       <c r="B178" s="1">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C178" t="s">
-        <v>454</v>
+        <v>350</v>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.15">
@@ -9476,10 +9482,10 @@
         <v>264</v>
       </c>
       <c r="B179" s="1">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C179" t="s">
-        <v>455</v>
+        <v>353</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.15">
@@ -9487,10 +9493,10 @@
         <v>264</v>
       </c>
       <c r="B180" s="1">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C180" t="s">
-        <v>456</v>
+        <v>354</v>
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.15">
@@ -9498,10 +9504,10 @@
         <v>264</v>
       </c>
       <c r="B181" s="1">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C181" t="s">
-        <v>457</v>
+        <v>406</v>
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.15">
@@ -9509,10 +9515,10 @@
         <v>264</v>
       </c>
       <c r="B182" s="1">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C182" t="s">
-        <v>458</v>
+        <v>407</v>
       </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.15">
@@ -9520,10 +9526,10 @@
         <v>264</v>
       </c>
       <c r="B183" s="1">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C183" t="s">
-        <v>459</v>
+        <v>410</v>
       </c>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.15">
@@ -9531,10 +9537,10 @@
         <v>264</v>
       </c>
       <c r="B184" s="1">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C184" t="s">
-        <v>460</v>
+        <v>411</v>
       </c>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.15">
@@ -9542,10 +9548,10 @@
         <v>264</v>
       </c>
       <c r="B185" s="1">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C185" t="s">
-        <v>461</v>
+        <v>437</v>
       </c>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.15">
@@ -9553,10 +9559,10 @@
         <v>264</v>
       </c>
       <c r="B186" s="1">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C186" t="s">
-        <v>462</v>
+        <v>438</v>
       </c>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.15">
@@ -9564,10 +9570,10 @@
         <v>264</v>
       </c>
       <c r="B187" s="1">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C187" t="s">
-        <v>463</v>
+        <v>441</v>
       </c>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.15">
@@ -9575,10 +9581,10 @@
         <v>264</v>
       </c>
       <c r="B188" s="1">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C188" t="s">
-        <v>464</v>
+        <v>442</v>
       </c>
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.15">
@@ -9586,10 +9592,10 @@
         <v>264</v>
       </c>
       <c r="B189" s="1">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C189" t="s">
-        <v>465</v>
+        <v>444</v>
       </c>
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.15">
@@ -9597,10 +9603,10 @@
         <v>264</v>
       </c>
       <c r="B190" s="1">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C190" t="s">
-        <v>466</v>
+        <v>445</v>
       </c>
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.15">
@@ -9608,10 +9614,10 @@
         <v>264</v>
       </c>
       <c r="B191" s="1">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C191" t="s">
-        <v>467</v>
+        <v>448</v>
       </c>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.15">
@@ -9619,10 +9625,10 @@
         <v>264</v>
       </c>
       <c r="B192" s="1">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C192" t="s">
-        <v>468</v>
+        <v>449</v>
       </c>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.15">
@@ -9630,10 +9636,10 @@
         <v>264</v>
       </c>
       <c r="B193" s="1">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C193" t="s">
-        <v>469</v>
+        <v>451</v>
       </c>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.15">
@@ -9641,10 +9647,10 @@
         <v>264</v>
       </c>
       <c r="B194" s="1">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C194" t="s">
-        <v>470</v>
+        <v>452</v>
       </c>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.15">
@@ -9652,10 +9658,10 @@
         <v>264</v>
       </c>
       <c r="B195" s="1">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C195" t="s">
-        <v>471</v>
+        <v>455</v>
       </c>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.15">
@@ -9663,10 +9669,10 @@
         <v>264</v>
       </c>
       <c r="B196" s="1">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C196" t="s">
-        <v>472</v>
+        <v>456</v>
       </c>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.15">
@@ -9674,10 +9680,10 @@
         <v>264</v>
       </c>
       <c r="B197" s="1">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C197" t="s">
-        <v>473</v>
+        <v>458</v>
       </c>
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.15">
@@ -9685,10 +9691,10 @@
         <v>264</v>
       </c>
       <c r="B198" s="1">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C198" t="s">
-        <v>474</v>
+        <v>459</v>
       </c>
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.15">
@@ -9696,10 +9702,10 @@
         <v>264</v>
       </c>
       <c r="B199" s="1">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C199" t="s">
-        <v>475</v>
+        <v>462</v>
       </c>
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.15">
@@ -9707,10 +9713,10 @@
         <v>264</v>
       </c>
       <c r="B200" s="1">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C200" t="s">
-        <v>476</v>
+        <v>463</v>
       </c>
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.15">
@@ -9718,10 +9724,10 @@
         <v>264</v>
       </c>
       <c r="B201" s="1">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C201" t="s">
-        <v>477</v>
+        <v>465</v>
       </c>
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.15">
@@ -9729,10 +9735,10 @@
         <v>264</v>
       </c>
       <c r="B202" s="1">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C202" t="s">
-        <v>478</v>
+        <v>466</v>
       </c>
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.15">
@@ -9740,10 +9746,10 @@
         <v>264</v>
       </c>
       <c r="B203" s="1">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C203" t="s">
-        <v>279</v>
+        <v>469</v>
       </c>
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.15">
@@ -9751,10 +9757,10 @@
         <v>264</v>
       </c>
       <c r="B204" s="1">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C204" t="s">
-        <v>280</v>
+        <v>470</v>
       </c>
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.15">
@@ -9762,10 +9768,10 @@
         <v>264</v>
       </c>
       <c r="B205" s="1">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C205" t="s">
-        <v>281</v>
+        <v>472</v>
       </c>
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.15">
@@ -9773,10 +9779,10 @@
         <v>264</v>
       </c>
       <c r="B206" s="1">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C206" t="s">
-        <v>282</v>
+        <v>473</v>
       </c>
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.15">
@@ -9784,10 +9790,10 @@
         <v>264</v>
       </c>
       <c r="B207" s="1">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C207" t="s">
-        <v>283</v>
+        <v>476</v>
       </c>
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.15">
@@ -9795,10 +9801,10 @@
         <v>264</v>
       </c>
       <c r="B208" s="1">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C208" t="s">
-        <v>284</v>
+        <v>477</v>
       </c>
     </row>
     <row r="209" spans="1:3" x14ac:dyDescent="0.15">
@@ -9809,7 +9815,7 @@
         <v>34</v>
       </c>
       <c r="C209" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.15">
@@ -9817,10 +9823,10 @@
         <v>264</v>
       </c>
       <c r="B210" s="1">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C210" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.15">
@@ -9828,10 +9834,10 @@
         <v>264</v>
       </c>
       <c r="B211" s="1">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C211" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.15">
@@ -9839,10 +9845,10 @@
         <v>264</v>
       </c>
       <c r="B212" s="1">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C212" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
     </row>
     <row r="213" spans="1:3" x14ac:dyDescent="0.15">
@@ -9853,7 +9859,7 @@
         <v>35</v>
       </c>
       <c r="C213" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
     </row>
     <row r="214" spans="1:3" x14ac:dyDescent="0.15">
@@ -9864,7 +9870,7 @@
         <v>35</v>
       </c>
       <c r="C214" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
     </row>
     <row r="215" spans="1:3" x14ac:dyDescent="0.15">
@@ -9875,7 +9881,7 @@
         <v>35</v>
       </c>
       <c r="C215" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="216" spans="1:3" x14ac:dyDescent="0.15">
@@ -9886,14 +9892,15 @@
         <v>35</v>
       </c>
       <c r="C216" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A1:C265">
-    <sortCondition ref="B1:B265"/>
+  <sortState ref="A1:C216">
+    <sortCondition ref="B1:B216"/>
   </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Baseboard_v0105 1)Fix power ok and clock sequence issue 2)Modify net name in source code top file according to schematic
</commit_message>
<xml_diff>
--- a/Baseboard/BBmapping.xlsx
+++ b/Baseboard/BBmapping.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
     <sheet name="Swap" sheetId="2" r:id="rId2"/>
-    <sheet name="Final" sheetId="3" r:id="rId3"/>
+    <sheet name="Final20150214" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1560" uniqueCount="484">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1849" uniqueCount="656">
   <si>
     <t>LOCATE COMP "DRV0_PWROK" SITE "M4" ;</t>
   </si>
@@ -1480,12 +1480,587 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>HDD25</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>HDD26</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>HDD27</t>
+  </si>
+  <si>
+    <t>HDD28</t>
+  </si>
+  <si>
+    <t>HDD29</t>
+  </si>
+  <si>
+    <t>HDD30</t>
+  </si>
+  <si>
+    <t>HDD31</t>
+  </si>
+  <si>
+    <t>HDD32</t>
+  </si>
+  <si>
+    <t>HDD33</t>
+  </si>
+  <si>
+    <t>HDD34</t>
+  </si>
+  <si>
+    <t>HDD35</t>
+  </si>
+  <si>
+    <t>HDD36</t>
+  </si>
+  <si>
+    <t>J25</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>J26</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>J27</t>
+  </si>
+  <si>
+    <t>J28</t>
+  </si>
+  <si>
+    <t>J29</t>
+  </si>
+  <si>
+    <t>J30</t>
+  </si>
+  <si>
+    <t>J31</t>
+  </si>
+  <si>
+    <t>J32</t>
+  </si>
+  <si>
+    <t>J33</t>
+  </si>
+  <si>
+    <t>J34</t>
+  </si>
+  <si>
+    <t>J35</t>
+  </si>
+  <si>
+    <t>J36</t>
+  </si>
+  <si>
+    <t>HDD49</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>HDD50</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>HDD51</t>
+  </si>
+  <si>
+    <t>HDD52</t>
+  </si>
+  <si>
+    <t>HDD53</t>
+  </si>
+  <si>
+    <t>HDD54</t>
+  </si>
+  <si>
+    <t>HDD55</t>
+  </si>
+  <si>
+    <t>HDD56</t>
+  </si>
+  <si>
+    <t>HDD57</t>
+  </si>
+  <si>
+    <t>HDD58</t>
+  </si>
+  <si>
+    <t>HDD59</t>
+  </si>
+  <si>
+    <t>HDD60</t>
+  </si>
+  <si>
+    <t>J1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>J2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>J3</t>
+  </si>
+  <si>
+    <t>J4</t>
+  </si>
+  <si>
+    <t>J5</t>
+  </si>
+  <si>
+    <t>J6</t>
+  </si>
+  <si>
+    <t>J7</t>
+  </si>
+  <si>
+    <t>J8</t>
+  </si>
+  <si>
+    <t>J9</t>
+  </si>
+  <si>
+    <t>J10</t>
+  </si>
+  <si>
+    <t>J11</t>
+  </si>
+  <si>
+    <t>J12</t>
+  </si>
+  <si>
+    <t>PE_RST_DRV0_A_L</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PE_RST_DRV1_A_L</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PE_RST_DRV2_A_L</t>
+  </si>
+  <si>
+    <t>PE_RST_DRV3_A_L</t>
+  </si>
+  <si>
+    <t>PE_RST_DRV4_A_L</t>
+  </si>
+  <si>
+    <t>PE_RST_DRV5_A_L</t>
+  </si>
+  <si>
+    <t>PE_RST_DRV6_A_L</t>
+  </si>
+  <si>
+    <t>PE_RST_DRV7_A_L</t>
+  </si>
+  <si>
+    <t>PE_RST_DRV8_A_L</t>
+  </si>
+  <si>
+    <t>PE_RST_DRV9_A_L</t>
+  </si>
+  <si>
+    <t>PE_RST_DRV10_A_L</t>
+  </si>
+  <si>
+    <t>PE_RST_DRV11_A_L</t>
+  </si>
+  <si>
+    <t>PE_RST_DRV0_B_L</t>
+  </si>
+  <si>
+    <t>PE_RST_DRV0_B_L</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PE_RST_DRV1_B_L</t>
+  </si>
+  <si>
+    <t>PE_RST_DRV1_B_L</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PE_RST_DRV2_B_L</t>
+  </si>
+  <si>
+    <t>PE_RST_DRV3_B_L</t>
+  </si>
+  <si>
+    <t>PE_RST_DRV4_B_L</t>
+  </si>
+  <si>
+    <t>PE_RST_DRV5_B_L</t>
+  </si>
+  <si>
+    <t>PE_RST_DRV6_B_L</t>
+  </si>
+  <si>
+    <t>PE_RST_DRV7_B_L</t>
+  </si>
+  <si>
+    <t>PE_RST_DRV8_B_L</t>
+  </si>
+  <si>
+    <t>PE_RST_DRV9_B_L</t>
+  </si>
+  <si>
+    <t>PE_RST_DRV10_B_L</t>
+  </si>
+  <si>
+    <t>PE_RST_DRV11_B_L</t>
+  </si>
+  <si>
+    <t>LOCATE COMP "DRV</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LOCATE COMP "PE_RST_DRV</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>_PWROK" SITE "Y1" ;</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>_PCIE_CLK_A_OE_L" SITE "W6" ;</t>
+    <t>PE_RST_DRV12_A_L</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PE_RST_DRV13_A_L</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PE_RST_DRV14_A_L</t>
+  </si>
+  <si>
+    <t>PE_RST_DRV15_A_L</t>
+  </si>
+  <si>
+    <t>PE_RST_DRV16_A_L</t>
+  </si>
+  <si>
+    <t>PE_RST_DRV18_A_L</t>
+  </si>
+  <si>
+    <t>PE_RST_DRV19_A_L</t>
+  </si>
+  <si>
+    <t>PE_RST_DRV20_A_L</t>
+  </si>
+  <si>
+    <t>PE_RST_DRV21_A_L</t>
+  </si>
+  <si>
+    <t>PE_RST_DRV22_A_L</t>
+  </si>
+  <si>
+    <t>PE_RST_DRV23_A_L</t>
+  </si>
+  <si>
+    <t>PE_RST_DRV12_B_L</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PE_RST_DRV13_B_L</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PE_RST_DRV14_B_L</t>
+  </si>
+  <si>
+    <t>PE_RST_DRV15_B_L</t>
+  </si>
+  <si>
+    <t>PE_RST_DRV16_B_L</t>
+  </si>
+  <si>
+    <t>PE_RST_DRV17_B_L</t>
+  </si>
+  <si>
+    <t>PE_RST_DRV18_B_L</t>
+  </si>
+  <si>
+    <t>PE_RST_DRV19_B_L</t>
+  </si>
+  <si>
+    <t>PE_RST_DRV20_B_L</t>
+  </si>
+  <si>
+    <t>PE_RST_DRV21_B_L</t>
+  </si>
+  <si>
+    <t>PE_RST_DRV22_B_L</t>
+  </si>
+  <si>
+    <t>PE_RST_DRV23_B_L</t>
+  </si>
+  <si>
+    <t>Net Name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PE_RST_DRV25_A_L</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PE_RST_DRV26_A_L</t>
+  </si>
+  <si>
+    <t>PE_RST_DRV27_A_L</t>
+  </si>
+  <si>
+    <t>PE_RST_DRV28_A_L</t>
+  </si>
+  <si>
+    <t>PE_RST_DRV29_A_L</t>
+  </si>
+  <si>
+    <t>PE_RST_DRV30_A_L</t>
+  </si>
+  <si>
+    <t>PE_RST_DRV31_A_L</t>
+  </si>
+  <si>
+    <t>PE_RST_DRV32_A_L</t>
+  </si>
+  <si>
+    <t>PE_RST_DRV33_A_L</t>
+  </si>
+  <si>
+    <t>PE_RST_DRV34_A_L</t>
+  </si>
+  <si>
+    <t>PE_RST_DRV35_A_L</t>
+  </si>
+  <si>
+    <t>PE_RST_DRV24_B_L</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PE_RST_DRV25_B_L</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PE_RST_DRV26_B_L</t>
+  </si>
+  <si>
+    <t>PE_RST_DRV27_B_L</t>
+  </si>
+  <si>
+    <t>PE_RST_DRV28_B_L</t>
+  </si>
+  <si>
+    <t>PE_RST_DRV29_B_L</t>
+  </si>
+  <si>
+    <t>PE_RST_DRV30_B_L</t>
+  </si>
+  <si>
+    <t>PE_RST_DRV31_B_L</t>
+  </si>
+  <si>
+    <t>PE_RST_DRV32_B_L</t>
+  </si>
+  <si>
+    <t>PE_RST_DRV33_B_L</t>
+  </si>
+  <si>
+    <t>PE_RST_DRV34_B_L</t>
+  </si>
+  <si>
+    <t>PE_RST_DRV35_B_L</t>
+  </si>
+  <si>
+    <t>PE_RST_DRV17_A_L</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PE_RST_DRV24_A_L</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>_A_L" SITE "P19" ;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>_A_L" SITE "T19" ;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>_A_L" SITE "R6" ;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>_A_L" SITE "D16" ;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>_A_L" SITE "J21" ;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>_A_L" SITE "U11" ;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>_A_L" SITE "H20" ;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>_A_L" SITE "T22" ;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>_A_L" SITE "U10" ;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>_A_L" SITE "AA11" ;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>_A_L" SITE "C17" ;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>_A_L" SITE "E8" ;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>_B_L" SITE "Y21" ;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>_B_L" SITE "U22" ;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>_B_L" SITE "T5" ;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>_B_L" SITE "D14" ;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>_B_L" SITE "M18" ;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>_B_L" SITE "T11" ;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>_B_L" SITE "E20" ;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>_B_L" SITE "T21" ;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>_B_L" SITE "Y6" ;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>_B_L" SITE "T10" ;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>_B_L" SITE "C16" ;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>_B_L" SITE "L6" ;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>_A_L" SITE "M5" ;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>_A_L" SITE "E6" ;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>_A_L" SITE "E14" ;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>_A_L" SITE "D22" ;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>_A_L" SITE "D19" ;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>_A_L" SITE "B15" ;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>_A_L" SITE "F16" ;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>_A_L" SITE "G11" ;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>_A_L" SITE "G10" ;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>_A_L" SITE "C8" ;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>_A_L" SITE "F8" ;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>_A_L" SITE "U3" ;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>_B_L" SITE "N5" ;</t>
+  </si>
+  <si>
+    <t>_B_L" SITE "D8" ;</t>
+  </si>
+  <si>
+    <t>_B_L" SITE "D17" ;</t>
+  </si>
+  <si>
+    <t>_B_L" SITE "E21" ;</t>
+  </si>
+  <si>
+    <t>_B_L" SITE "C21" ;</t>
+  </si>
+  <si>
+    <t>_B_L" SITE "H17" ;</t>
+  </si>
+  <si>
+    <t>_B_L" SITE "E17" ;</t>
+  </si>
+  <si>
+    <t>_B_L" SITE "C19" ;</t>
+  </si>
+  <si>
+    <t>_B_L" SITE "F10" ;</t>
+  </si>
+  <si>
+    <t>_B_L" SITE "C5" ;</t>
+  </si>
+  <si>
+    <t>_B_L" SITE "B4" ;</t>
+  </si>
+  <si>
+    <t>_B_L" SITE "R2" ;</t>
   </si>
 </sst>
 </file>
@@ -7508,15 +8083,24 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C216"/>
+  <dimension ref="A1:I270"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A230" workbookViewId="0">
+      <selection activeCell="J271" sqref="J271"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="18.375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.25" style="1" customWidth="1"/>
+    <col min="1" max="1" width="26.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.5" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="35" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="18.375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="3.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="19" width="17.25" bestFit="1" customWidth="1"/>
+    <col min="20" max="21" width="18.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.15">
@@ -7568,10 +8152,10 @@
         <v>264</v>
       </c>
       <c r="B5" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>483</v>
+        <v>386</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.15">
@@ -7579,10 +8163,10 @@
         <v>264</v>
       </c>
       <c r="B6" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>268</v>
+        <v>387</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.15">
@@ -7590,10 +8174,10 @@
         <v>264</v>
       </c>
       <c r="B7" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>271</v>
+        <v>388</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.15">
@@ -7604,7 +8188,7 @@
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>386</v>
+        <v>389</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.15">
@@ -7612,10 +8196,10 @@
         <v>264</v>
       </c>
       <c r="B9" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>387</v>
+        <v>390</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.15">
@@ -7623,10 +8207,10 @@
         <v>264</v>
       </c>
       <c r="B10" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C10" t="s">
-        <v>388</v>
+        <v>391</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.15">
@@ -7634,10 +8218,10 @@
         <v>264</v>
       </c>
       <c r="B11" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C11" t="s">
-        <v>389</v>
+        <v>392</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.15">
@@ -7645,10 +8229,10 @@
         <v>264</v>
       </c>
       <c r="B12" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C12" t="s">
-        <v>274</v>
+        <v>393</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.15">
@@ -7656,10 +8240,10 @@
         <v>264</v>
       </c>
       <c r="B13" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C13" t="s">
-        <v>275</v>
+        <v>394</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.15">
@@ -7667,10 +8251,10 @@
         <v>264</v>
       </c>
       <c r="B14" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C14" t="s">
-        <v>278</v>
+        <v>395</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.15">
@@ -7678,10 +8262,10 @@
         <v>264</v>
       </c>
       <c r="B15" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C15" t="s">
-        <v>390</v>
+        <v>396</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.15">
@@ -7689,10 +8273,10 @@
         <v>264</v>
       </c>
       <c r="B16" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C16" t="s">
-        <v>391</v>
+        <v>397</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.15">
@@ -7700,10 +8284,10 @@
         <v>264</v>
       </c>
       <c r="B17" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C17" t="s">
-        <v>392</v>
+        <v>398</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.15">
@@ -7711,10 +8295,10 @@
         <v>264</v>
       </c>
       <c r="B18" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C18" t="s">
-        <v>393</v>
+        <v>399</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.15">
@@ -7722,10 +8306,10 @@
         <v>264</v>
       </c>
       <c r="B19" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C19" t="s">
-        <v>351</v>
+        <v>400</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.15">
@@ -7733,10 +8317,10 @@
         <v>264</v>
       </c>
       <c r="B20" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C20" t="s">
-        <v>352</v>
+        <v>401</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.15">
@@ -7744,10 +8328,10 @@
         <v>264</v>
       </c>
       <c r="B21" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C21" t="s">
-        <v>355</v>
+        <v>402</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.15">
@@ -7755,10 +8339,10 @@
         <v>264</v>
       </c>
       <c r="B22" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C22" t="s">
-        <v>394</v>
+        <v>403</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.15">
@@ -7766,10 +8350,10 @@
         <v>264</v>
       </c>
       <c r="B23" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C23" t="s">
-        <v>395</v>
+        <v>404</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.15">
@@ -7777,10 +8361,10 @@
         <v>264</v>
       </c>
       <c r="B24" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C24" t="s">
-        <v>396</v>
+        <v>405</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.15">
@@ -7788,10 +8372,10 @@
         <v>264</v>
       </c>
       <c r="B25" s="1">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C25" t="s">
-        <v>397</v>
+        <v>413</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.15">
@@ -7799,10 +8383,10 @@
         <v>264</v>
       </c>
       <c r="B26" s="1">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C26" t="s">
-        <v>408</v>
+        <v>414</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.15">
@@ -7810,10 +8394,10 @@
         <v>264</v>
       </c>
       <c r="B27" s="1">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C27" t="s">
-        <v>409</v>
+        <v>415</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.15">
@@ -7821,10 +8405,10 @@
         <v>264</v>
       </c>
       <c r="B28" s="1">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C28" t="s">
-        <v>412</v>
+        <v>416</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.15">
@@ -7832,10 +8416,10 @@
         <v>264</v>
       </c>
       <c r="B29" s="1">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C29" t="s">
-        <v>398</v>
+        <v>417</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.15">
@@ -7843,10 +8427,10 @@
         <v>264</v>
       </c>
       <c r="B30" s="1">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C30" t="s">
-        <v>399</v>
+        <v>418</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.15">
@@ -7854,10 +8438,10 @@
         <v>264</v>
       </c>
       <c r="B31" s="1">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C31" t="s">
-        <v>400</v>
+        <v>419</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.15">
@@ -7865,10 +8449,10 @@
         <v>264</v>
       </c>
       <c r="B32" s="1">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C32" t="s">
-        <v>401</v>
+        <v>420</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.15">
@@ -7876,10 +8460,10 @@
         <v>264</v>
       </c>
       <c r="B33" s="1">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C33" t="s">
-        <v>439</v>
+        <v>421</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.15">
@@ -7887,10 +8471,10 @@
         <v>264</v>
       </c>
       <c r="B34" s="1">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C34" t="s">
-        <v>440</v>
+        <v>422</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.15">
@@ -7898,10 +8482,10 @@
         <v>264</v>
       </c>
       <c r="B35" s="1">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C35" t="s">
-        <v>443</v>
+        <v>423</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.15">
@@ -7909,10 +8493,10 @@
         <v>264</v>
       </c>
       <c r="B36" s="1">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C36" t="s">
-        <v>402</v>
+        <v>424</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.15">
@@ -7920,10 +8504,10 @@
         <v>264</v>
       </c>
       <c r="B37" s="1">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C37" t="s">
-        <v>403</v>
+        <v>425</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.15">
@@ -7931,10 +8515,10 @@
         <v>264</v>
       </c>
       <c r="B38" s="1">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C38" t="s">
-        <v>404</v>
+        <v>426</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.15">
@@ -7942,10 +8526,10 @@
         <v>264</v>
       </c>
       <c r="B39" s="1">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C39" t="s">
-        <v>405</v>
+        <v>427</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.15">
@@ -7953,10 +8537,10 @@
         <v>264</v>
       </c>
       <c r="B40" s="1">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C40" t="s">
-        <v>446</v>
+        <v>428</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.15">
@@ -7964,10 +8548,10 @@
         <v>264</v>
       </c>
       <c r="B41" s="1">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C41" t="s">
-        <v>447</v>
+        <v>429</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.15">
@@ -7975,10 +8559,10 @@
         <v>264</v>
       </c>
       <c r="B42" s="1">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C42" t="s">
-        <v>450</v>
+        <v>430</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.15">
@@ -7986,10 +8570,10 @@
         <v>264</v>
       </c>
       <c r="B43" s="1">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C43" t="s">
-        <v>413</v>
+        <v>431</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.15">
@@ -7997,10 +8581,10 @@
         <v>264</v>
       </c>
       <c r="B44" s="1">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C44" t="s">
-        <v>414</v>
+        <v>432</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.15">
@@ -8008,10 +8592,10 @@
         <v>264</v>
       </c>
       <c r="B45" s="1">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C45" t="s">
-        <v>415</v>
+        <v>433</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.15">
@@ -8019,10 +8603,10 @@
         <v>264</v>
       </c>
       <c r="B46" s="1">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C46" t="s">
-        <v>416</v>
+        <v>434</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.15">
@@ -8030,10 +8614,10 @@
         <v>264</v>
       </c>
       <c r="B47" s="1">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C47" t="s">
-        <v>453</v>
+        <v>435</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.15">
@@ -8041,10 +8625,10 @@
         <v>264</v>
       </c>
       <c r="B48" s="1">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C48" t="s">
-        <v>454</v>
+        <v>436</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.15">
@@ -8052,10 +8636,10 @@
         <v>264</v>
       </c>
       <c r="B49" s="1">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C49" t="s">
-        <v>457</v>
+        <v>293</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.15">
@@ -8063,10 +8647,10 @@
         <v>264</v>
       </c>
       <c r="B50" s="1">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C50" t="s">
-        <v>417</v>
+        <v>294</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.15">
@@ -8074,10 +8658,10 @@
         <v>264</v>
       </c>
       <c r="B51" s="1">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C51" t="s">
-        <v>418</v>
+        <v>295</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.15">
@@ -8085,10 +8669,10 @@
         <v>264</v>
       </c>
       <c r="B52" s="1">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C52" t="s">
-        <v>419</v>
+        <v>296</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.15">
@@ -8096,10 +8680,10 @@
         <v>264</v>
       </c>
       <c r="B53" s="1">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C53" t="s">
-        <v>420</v>
+        <v>297</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.15">
@@ -8107,10 +8691,10 @@
         <v>264</v>
       </c>
       <c r="B54" s="1">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C54" t="s">
-        <v>460</v>
+        <v>298</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.15">
@@ -8118,10 +8702,10 @@
         <v>264</v>
       </c>
       <c r="B55" s="1">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C55" t="s">
-        <v>461</v>
+        <v>299</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.15">
@@ -8129,10 +8713,10 @@
         <v>264</v>
       </c>
       <c r="B56" s="1">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="C56" t="s">
-        <v>464</v>
+        <v>300</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.15">
@@ -8140,10 +8724,10 @@
         <v>264</v>
       </c>
       <c r="B57" s="1">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C57" t="s">
-        <v>421</v>
+        <v>301</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.15">
@@ -8151,10 +8735,10 @@
         <v>264</v>
       </c>
       <c r="B58" s="1">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C58" t="s">
-        <v>422</v>
+        <v>302</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.15">
@@ -8162,10 +8746,10 @@
         <v>264</v>
       </c>
       <c r="B59" s="1">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C59" t="s">
-        <v>423</v>
+        <v>303</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.15">
@@ -8173,10 +8757,10 @@
         <v>264</v>
       </c>
       <c r="B60" s="1">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C60" t="s">
-        <v>424</v>
+        <v>304</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.15">
@@ -8184,10 +8768,10 @@
         <v>264</v>
       </c>
       <c r="B61" s="1">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C61" t="s">
-        <v>467</v>
+        <v>305</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.15">
@@ -8195,10 +8779,10 @@
         <v>264</v>
       </c>
       <c r="B62" s="1">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C62" t="s">
-        <v>468</v>
+        <v>306</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.15">
@@ -8206,10 +8790,10 @@
         <v>264</v>
       </c>
       <c r="B63" s="1">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C63" t="s">
-        <v>471</v>
+        <v>307</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.15">
@@ -8217,10 +8801,10 @@
         <v>264</v>
       </c>
       <c r="B64" s="1">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C64" t="s">
-        <v>425</v>
+        <v>308</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.15">
@@ -8228,10 +8812,10 @@
         <v>264</v>
       </c>
       <c r="B65" s="1">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C65" t="s">
-        <v>426</v>
+        <v>309</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.15">
@@ -8239,10 +8823,10 @@
         <v>264</v>
       </c>
       <c r="B66" s="1">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C66" t="s">
-        <v>427</v>
+        <v>310</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.15">
@@ -8250,10 +8834,10 @@
         <v>264</v>
       </c>
       <c r="B67" s="1">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C67" t="s">
-        <v>428</v>
+        <v>311</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.15">
@@ -8261,10 +8845,10 @@
         <v>264</v>
       </c>
       <c r="B68" s="1">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C68" t="s">
-        <v>474</v>
+        <v>312</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.15">
@@ -8272,10 +8856,10 @@
         <v>264</v>
       </c>
       <c r="B69" s="1">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C69" t="s">
-        <v>475</v>
+        <v>313</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.15">
@@ -8283,10 +8867,10 @@
         <v>264</v>
       </c>
       <c r="B70" s="1">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C70" t="s">
-        <v>478</v>
+        <v>314</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.15">
@@ -8294,10 +8878,10 @@
         <v>264</v>
       </c>
       <c r="B71" s="1">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C71" t="s">
-        <v>429</v>
+        <v>315</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.15">
@@ -8305,10 +8889,10 @@
         <v>264</v>
       </c>
       <c r="B72" s="1">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C72" t="s">
-        <v>430</v>
+        <v>316</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.15">
@@ -8316,10 +8900,10 @@
         <v>264</v>
       </c>
       <c r="B73" s="1">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C73" t="s">
-        <v>431</v>
+        <v>317</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.15">
@@ -8327,10 +8911,10 @@
         <v>264</v>
       </c>
       <c r="B74" s="1">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C74" t="s">
-        <v>432</v>
+        <v>318</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.15">
@@ -8338,10 +8922,10 @@
         <v>264</v>
       </c>
       <c r="B75" s="1">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C75" t="s">
-        <v>281</v>
+        <v>319</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.15">
@@ -8349,10 +8933,10 @@
         <v>264</v>
       </c>
       <c r="B76" s="1">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C76" t="s">
-        <v>282</v>
+        <v>320</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.15">
@@ -8360,10 +8944,10 @@
         <v>264</v>
       </c>
       <c r="B77" s="1">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C77" t="s">
-        <v>285</v>
+        <v>321</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.15">
@@ -8371,10 +8955,10 @@
         <v>264</v>
       </c>
       <c r="B78" s="1">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="C78" t="s">
-        <v>433</v>
+        <v>322</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.15">
@@ -8382,10 +8966,10 @@
         <v>264</v>
       </c>
       <c r="B79" s="1">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="C79" t="s">
-        <v>434</v>
+        <v>323</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.15">
@@ -8393,10 +8977,10 @@
         <v>264</v>
       </c>
       <c r="B80" s="1">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="C80" t="s">
-        <v>435</v>
+        <v>324</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.15">
@@ -8404,10 +8988,10 @@
         <v>264</v>
       </c>
       <c r="B81" s="1">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="C81" t="s">
-        <v>436</v>
+        <v>325</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.15">
@@ -8415,10 +8999,10 @@
         <v>264</v>
       </c>
       <c r="B82" s="1">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="C82" t="s">
-        <v>288</v>
+        <v>326</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.15">
@@ -8426,10 +9010,10 @@
         <v>264</v>
       </c>
       <c r="B83" s="1">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="C83" t="s">
-        <v>289</v>
+        <v>327</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.15">
@@ -8437,10 +9021,10 @@
         <v>264</v>
       </c>
       <c r="B84" s="1">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="C84" t="s">
-        <v>482</v>
+        <v>328</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.15">
@@ -8448,10 +9032,10 @@
         <v>264</v>
       </c>
       <c r="B85" s="1">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C85" t="s">
-        <v>293</v>
+        <v>329</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.15">
@@ -8459,10 +9043,10 @@
         <v>264</v>
       </c>
       <c r="B86" s="1">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C86" t="s">
-        <v>294</v>
+        <v>330</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.15">
@@ -8470,10 +9054,10 @@
         <v>264</v>
       </c>
       <c r="B87" s="1">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C87" t="s">
-        <v>295</v>
+        <v>331</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.15">
@@ -8481,10 +9065,10 @@
         <v>264</v>
       </c>
       <c r="B88" s="1">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C88" t="s">
-        <v>296</v>
+        <v>332</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.15">
@@ -8492,10 +9076,10 @@
         <v>264</v>
       </c>
       <c r="B89" s="1">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C89" t="s">
-        <v>297</v>
+        <v>333</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.15">
@@ -8503,10 +9087,10 @@
         <v>264</v>
       </c>
       <c r="B90" s="1">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C90" t="s">
-        <v>298</v>
+        <v>334</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.15">
@@ -8514,10 +9098,10 @@
         <v>264</v>
       </c>
       <c r="B91" s="1">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="C91" t="s">
-        <v>299</v>
+        <v>335</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.15">
@@ -8525,10 +9109,10 @@
         <v>264</v>
       </c>
       <c r="B92" s="1">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C92" t="s">
-        <v>300</v>
+        <v>336</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.15">
@@ -8536,10 +9120,10 @@
         <v>264</v>
       </c>
       <c r="B93" s="1">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C93" t="s">
-        <v>301</v>
+        <v>337</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.15">
@@ -8547,10 +9131,10 @@
         <v>264</v>
       </c>
       <c r="B94" s="1">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C94" t="s">
-        <v>302</v>
+        <v>338</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.15">
@@ -8558,10 +9142,10 @@
         <v>264</v>
       </c>
       <c r="B95" s="1">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C95" t="s">
-        <v>303</v>
+        <v>339</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.15">
@@ -8569,10 +9153,10 @@
         <v>264</v>
       </c>
       <c r="B96" s="1">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C96" t="s">
-        <v>304</v>
+        <v>340</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.15">
@@ -8580,10 +9164,10 @@
         <v>264</v>
       </c>
       <c r="B97" s="1">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C97" t="s">
-        <v>305</v>
+        <v>341</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.15">
@@ -8591,10 +9175,10 @@
         <v>264</v>
       </c>
       <c r="B98" s="1">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="C98" t="s">
-        <v>306</v>
+        <v>342</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.15">
@@ -8602,10 +9186,10 @@
         <v>264</v>
       </c>
       <c r="B99" s="1">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C99" t="s">
-        <v>307</v>
+        <v>343</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.15">
@@ -8613,10 +9197,10 @@
         <v>264</v>
       </c>
       <c r="B100" s="1">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C100" t="s">
-        <v>308</v>
+        <v>344</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.15">
@@ -8624,10 +9208,10 @@
         <v>264</v>
       </c>
       <c r="B101" s="1">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C101" t="s">
-        <v>309</v>
+        <v>345</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.15">
@@ -8635,10 +9219,10 @@
         <v>264</v>
       </c>
       <c r="B102" s="1">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C102" t="s">
-        <v>310</v>
+        <v>346</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.15">
@@ -8646,10 +9230,10 @@
         <v>264</v>
       </c>
       <c r="B103" s="1">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C103" t="s">
-        <v>311</v>
+        <v>347</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.15">
@@ -8657,10 +9241,10 @@
         <v>264</v>
       </c>
       <c r="B104" s="1">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C104" t="s">
-        <v>312</v>
+        <v>348</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.15">
@@ -8668,10 +9252,10 @@
         <v>264</v>
       </c>
       <c r="B105" s="1">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="C105" t="s">
-        <v>313</v>
+        <v>356</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.15">
@@ -8679,10 +9263,10 @@
         <v>264</v>
       </c>
       <c r="B106" s="1">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C106" t="s">
-        <v>314</v>
+        <v>357</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.15">
@@ -8690,10 +9274,10 @@
         <v>264</v>
       </c>
       <c r="B107" s="1">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C107" t="s">
-        <v>315</v>
+        <v>358</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.15">
@@ -8701,10 +9285,10 @@
         <v>264</v>
       </c>
       <c r="B108" s="1">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C108" t="s">
-        <v>316</v>
+        <v>359</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.15">
@@ -8712,10 +9296,10 @@
         <v>264</v>
       </c>
       <c r="B109" s="1">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C109" t="s">
-        <v>317</v>
+        <v>360</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.15">
@@ -8723,10 +9307,10 @@
         <v>264</v>
       </c>
       <c r="B110" s="1">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C110" t="s">
-        <v>318</v>
+        <v>361</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.15">
@@ -8734,10 +9318,10 @@
         <v>264</v>
       </c>
       <c r="B111" s="1">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C111" t="s">
-        <v>319</v>
+        <v>362</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.15">
@@ -8745,10 +9329,10 @@
         <v>264</v>
       </c>
       <c r="B112" s="1">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="C112" t="s">
-        <v>320</v>
+        <v>363</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.15">
@@ -8756,10 +9340,10 @@
         <v>264</v>
       </c>
       <c r="B113" s="1">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="C113" t="s">
-        <v>321</v>
+        <v>364</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.15">
@@ -8767,10 +9351,10 @@
         <v>264</v>
       </c>
       <c r="B114" s="1">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="C114" t="s">
-        <v>322</v>
+        <v>365</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.15">
@@ -8778,10 +9362,10 @@
         <v>264</v>
       </c>
       <c r="B115" s="1">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="C115" t="s">
-        <v>323</v>
+        <v>366</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.15">
@@ -8789,10 +9373,10 @@
         <v>264</v>
       </c>
       <c r="B116" s="1">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="C116" t="s">
-        <v>324</v>
+        <v>367</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.15">
@@ -8800,10 +9384,10 @@
         <v>264</v>
       </c>
       <c r="B117" s="1">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="C117" t="s">
-        <v>325</v>
+        <v>368</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.15">
@@ -8811,10 +9395,10 @@
         <v>264</v>
       </c>
       <c r="B118" s="1">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="C118" t="s">
-        <v>326</v>
+        <v>369</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.15">
@@ -8822,10 +9406,10 @@
         <v>264</v>
       </c>
       <c r="B119" s="1">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="C119" t="s">
-        <v>327</v>
+        <v>370</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.15">
@@ -8833,10 +9417,10 @@
         <v>264</v>
       </c>
       <c r="B120" s="1">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C120" t="s">
-        <v>328</v>
+        <v>371</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.15">
@@ -8844,10 +9428,10 @@
         <v>264</v>
       </c>
       <c r="B121" s="1">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C121" t="s">
-        <v>329</v>
+        <v>372</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.15">
@@ -8855,10 +9439,10 @@
         <v>264</v>
       </c>
       <c r="B122" s="1">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C122" t="s">
-        <v>330</v>
+        <v>373</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.15">
@@ -8866,10 +9450,10 @@
         <v>264</v>
       </c>
       <c r="B123" s="1">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C123" t="s">
-        <v>331</v>
+        <v>374</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.15">
@@ -8877,10 +9461,10 @@
         <v>264</v>
       </c>
       <c r="B124" s="1">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C124" t="s">
-        <v>332</v>
+        <v>375</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.15">
@@ -8888,10 +9472,10 @@
         <v>264</v>
       </c>
       <c r="B125" s="1">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C125" t="s">
-        <v>333</v>
+        <v>376</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.15">
@@ -8899,10 +9483,10 @@
         <v>264</v>
       </c>
       <c r="B126" s="1">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="C126" t="s">
-        <v>334</v>
+        <v>377</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.15">
@@ -8910,10 +9494,10 @@
         <v>264</v>
       </c>
       <c r="B127" s="1">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="C127" t="s">
-        <v>335</v>
+        <v>378</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.15">
@@ -8921,10 +9505,10 @@
         <v>264</v>
       </c>
       <c r="B128" s="1">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="C128" t="s">
-        <v>336</v>
+        <v>379</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.15">
@@ -8932,10 +9516,10 @@
         <v>264</v>
       </c>
       <c r="B129" s="1">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="C129" t="s">
-        <v>337</v>
+        <v>380</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.15">
@@ -8943,10 +9527,10 @@
         <v>264</v>
       </c>
       <c r="B130" s="1">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="C130" t="s">
-        <v>338</v>
+        <v>381</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.15">
@@ -8954,10 +9538,10 @@
         <v>264</v>
       </c>
       <c r="B131" s="1">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="C131" t="s">
-        <v>339</v>
+        <v>382</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.15">
@@ -8965,21 +9549,21 @@
         <v>264</v>
       </c>
       <c r="B132" s="1">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="C132" t="s">
-        <v>340</v>
+        <v>479</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A133" t="s">
-        <v>264</v>
+        <v>481</v>
       </c>
       <c r="B133" s="1">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="C133" t="s">
-        <v>341</v>
+        <v>265</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.15">
@@ -8987,10 +9571,10 @@
         <v>264</v>
       </c>
       <c r="B134" s="1">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="C134" t="s">
-        <v>342</v>
+        <v>266</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.15">
@@ -8998,10 +9582,10 @@
         <v>264</v>
       </c>
       <c r="B135" s="1">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="C135" t="s">
-        <v>343</v>
+        <v>267</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.15">
@@ -9009,10 +9593,10 @@
         <v>264</v>
       </c>
       <c r="B136" s="1">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="C136" t="s">
-        <v>344</v>
+        <v>268</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.15">
@@ -9020,10 +9604,10 @@
         <v>264</v>
       </c>
       <c r="B137" s="1">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="C137" t="s">
-        <v>345</v>
+        <v>269</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.15">
@@ -9031,10 +9615,10 @@
         <v>264</v>
       </c>
       <c r="B138" s="1">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="C138" t="s">
-        <v>346</v>
+        <v>270</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.15">
@@ -9042,10 +9626,10 @@
         <v>264</v>
       </c>
       <c r="B139" s="1">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="C139" t="s">
-        <v>347</v>
+        <v>271</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.15">
@@ -9053,10 +9637,10 @@
         <v>264</v>
       </c>
       <c r="B140" s="1">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="C140" t="s">
-        <v>348</v>
+        <v>272</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.15">
@@ -9064,10 +9648,10 @@
         <v>264</v>
       </c>
       <c r="B141" s="1">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="C141" t="s">
-        <v>356</v>
+        <v>273</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.15">
@@ -9075,10 +9659,10 @@
         <v>264</v>
       </c>
       <c r="B142" s="1">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="C142" t="s">
-        <v>357</v>
+        <v>274</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.15">
@@ -9086,10 +9670,10 @@
         <v>264</v>
       </c>
       <c r="B143" s="1">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="C143" t="s">
-        <v>358</v>
+        <v>275</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.15">
@@ -9097,10 +9681,10 @@
         <v>264</v>
       </c>
       <c r="B144" s="1">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="C144" t="s">
-        <v>359</v>
+        <v>276</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.15">
@@ -9108,10 +9692,10 @@
         <v>264</v>
       </c>
       <c r="B145" s="1">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="C145" t="s">
-        <v>360</v>
+        <v>277</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.15">
@@ -9119,10 +9703,10 @@
         <v>264</v>
       </c>
       <c r="B146" s="1">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="C146" t="s">
-        <v>361</v>
+        <v>278</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.15">
@@ -9130,10 +9714,10 @@
         <v>264</v>
       </c>
       <c r="B147" s="1">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="C147" t="s">
-        <v>362</v>
+        <v>349</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.15">
@@ -9141,10 +9725,10 @@
         <v>264</v>
       </c>
       <c r="B148" s="1">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="C148" t="s">
-        <v>363</v>
+        <v>350</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.15">
@@ -9152,10 +9736,10 @@
         <v>264</v>
       </c>
       <c r="B149" s="1">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="C149" t="s">
-        <v>364</v>
+        <v>351</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.15">
@@ -9163,10 +9747,10 @@
         <v>264</v>
       </c>
       <c r="B150" s="1">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="C150" t="s">
-        <v>365</v>
+        <v>352</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.15">
@@ -9174,10 +9758,10 @@
         <v>264</v>
       </c>
       <c r="B151" s="1">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="C151" t="s">
-        <v>366</v>
+        <v>353</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.15">
@@ -9185,10 +9769,10 @@
         <v>264</v>
       </c>
       <c r="B152" s="1">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="C152" t="s">
-        <v>367</v>
+        <v>354</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.15">
@@ -9196,10 +9780,10 @@
         <v>264</v>
       </c>
       <c r="B153" s="1">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="C153" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.15">
@@ -9207,10 +9791,10 @@
         <v>264</v>
       </c>
       <c r="B154" s="1">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="C154" t="s">
-        <v>369</v>
+        <v>406</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.15">
@@ -9218,10 +9802,10 @@
         <v>264</v>
       </c>
       <c r="B155" s="1">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="C155" t="s">
-        <v>370</v>
+        <v>407</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.15">
@@ -9229,10 +9813,10 @@
         <v>264</v>
       </c>
       <c r="B156" s="1">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="C156" t="s">
-        <v>371</v>
+        <v>408</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.15">
@@ -9240,10 +9824,10 @@
         <v>264</v>
       </c>
       <c r="B157" s="1">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="C157" t="s">
-        <v>372</v>
+        <v>409</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.15">
@@ -9251,10 +9835,10 @@
         <v>264</v>
       </c>
       <c r="B158" s="1">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="C158" t="s">
-        <v>373</v>
+        <v>410</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.15">
@@ -9262,10 +9846,10 @@
         <v>264</v>
       </c>
       <c r="B159" s="1">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="C159" t="s">
-        <v>374</v>
+        <v>411</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.15">
@@ -9273,10 +9857,10 @@
         <v>264</v>
       </c>
       <c r="B160" s="1">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="C160" t="s">
-        <v>375</v>
+        <v>412</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.15">
@@ -9284,10 +9868,10 @@
         <v>264</v>
       </c>
       <c r="B161" s="1">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="C161" t="s">
-        <v>376</v>
+        <v>437</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.15">
@@ -9295,10 +9879,10 @@
         <v>264</v>
       </c>
       <c r="B162" s="1">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="C162" t="s">
-        <v>377</v>
+        <v>438</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.15">
@@ -9306,10 +9890,10 @@
         <v>264</v>
       </c>
       <c r="B163" s="1">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="C163" t="s">
-        <v>378</v>
+        <v>439</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.15">
@@ -9317,10 +9901,10 @@
         <v>264</v>
       </c>
       <c r="B164" s="1">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="C164" t="s">
-        <v>379</v>
+        <v>440</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.15">
@@ -9328,10 +9912,10 @@
         <v>264</v>
       </c>
       <c r="B165" s="1">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="C165" t="s">
-        <v>380</v>
+        <v>441</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.15">
@@ -9339,10 +9923,10 @@
         <v>264</v>
       </c>
       <c r="B166" s="1">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="C166" t="s">
-        <v>381</v>
+        <v>442</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.15">
@@ -9350,10 +9934,10 @@
         <v>264</v>
       </c>
       <c r="B167" s="1">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="C167" t="s">
-        <v>382</v>
+        <v>443</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.15">
@@ -9361,21 +9945,21 @@
         <v>264</v>
       </c>
       <c r="B168" s="1">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="C168" t="s">
-        <v>479</v>
+        <v>444</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A169" t="s">
-        <v>481</v>
+        <v>264</v>
       </c>
       <c r="B169" s="1">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="C169" t="s">
-        <v>265</v>
+        <v>445</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.15">
@@ -9383,10 +9967,10 @@
         <v>264</v>
       </c>
       <c r="B170" s="1">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="C170" t="s">
-        <v>266</v>
+        <v>446</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.15">
@@ -9394,10 +9978,10 @@
         <v>264</v>
       </c>
       <c r="B171" s="1">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="C171" t="s">
-        <v>269</v>
+        <v>447</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.15">
@@ -9405,10 +9989,10 @@
         <v>264</v>
       </c>
       <c r="B172" s="1">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="C172" t="s">
-        <v>270</v>
+        <v>448</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.15">
@@ -9416,10 +10000,10 @@
         <v>264</v>
       </c>
       <c r="B173" s="1">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="C173" t="s">
-        <v>272</v>
+        <v>449</v>
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.15">
@@ -9427,10 +10011,10 @@
         <v>264</v>
       </c>
       <c r="B174" s="1">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="C174" t="s">
-        <v>273</v>
+        <v>450</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.15">
@@ -9438,10 +10022,10 @@
         <v>264</v>
       </c>
       <c r="B175" s="1">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C175" t="s">
-        <v>276</v>
+        <v>451</v>
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.15">
@@ -9449,10 +10033,10 @@
         <v>264</v>
       </c>
       <c r="B176" s="1">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C176" t="s">
-        <v>277</v>
+        <v>452</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.15">
@@ -9460,10 +10044,10 @@
         <v>264</v>
       </c>
       <c r="B177" s="1">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="C177" t="s">
-        <v>349</v>
+        <v>453</v>
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.15">
@@ -9471,10 +10055,10 @@
         <v>264</v>
       </c>
       <c r="B178" s="1">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="C178" t="s">
-        <v>350</v>
+        <v>454</v>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.15">
@@ -9482,10 +10066,10 @@
         <v>264</v>
       </c>
       <c r="B179" s="1">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="C179" t="s">
-        <v>353</v>
+        <v>455</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.15">
@@ -9493,10 +10077,10 @@
         <v>264</v>
       </c>
       <c r="B180" s="1">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="C180" t="s">
-        <v>354</v>
+        <v>456</v>
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.15">
@@ -9504,10 +10088,10 @@
         <v>264</v>
       </c>
       <c r="B181" s="1">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C181" t="s">
-        <v>406</v>
+        <v>457</v>
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.15">
@@ -9515,10 +10099,10 @@
         <v>264</v>
       </c>
       <c r="B182" s="1">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="C182" t="s">
-        <v>407</v>
+        <v>458</v>
       </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.15">
@@ -9526,10 +10110,10 @@
         <v>264</v>
       </c>
       <c r="B183" s="1">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="C183" t="s">
-        <v>410</v>
+        <v>459</v>
       </c>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.15">
@@ -9537,10 +10121,10 @@
         <v>264</v>
       </c>
       <c r="B184" s="1">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="C184" t="s">
-        <v>411</v>
+        <v>460</v>
       </c>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.15">
@@ -9548,10 +10132,10 @@
         <v>264</v>
       </c>
       <c r="B185" s="1">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C185" t="s">
-        <v>437</v>
+        <v>461</v>
       </c>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.15">
@@ -9559,10 +10143,10 @@
         <v>264</v>
       </c>
       <c r="B186" s="1">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C186" t="s">
-        <v>438</v>
+        <v>462</v>
       </c>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.15">
@@ -9570,10 +10154,10 @@
         <v>264</v>
       </c>
       <c r="B187" s="1">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C187" t="s">
-        <v>441</v>
+        <v>463</v>
       </c>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.15">
@@ -9581,10 +10165,10 @@
         <v>264</v>
       </c>
       <c r="B188" s="1">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C188" t="s">
-        <v>442</v>
+        <v>464</v>
       </c>
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.15">
@@ -9592,10 +10176,10 @@
         <v>264</v>
       </c>
       <c r="B189" s="1">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C189" t="s">
-        <v>444</v>
+        <v>465</v>
       </c>
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.15">
@@ -9603,10 +10187,10 @@
         <v>264</v>
       </c>
       <c r="B190" s="1">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C190" t="s">
-        <v>445</v>
+        <v>466</v>
       </c>
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.15">
@@ -9614,10 +10198,10 @@
         <v>264</v>
       </c>
       <c r="B191" s="1">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C191" t="s">
-        <v>448</v>
+        <v>467</v>
       </c>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.15">
@@ -9625,10 +10209,10 @@
         <v>264</v>
       </c>
       <c r="B192" s="1">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C192" t="s">
-        <v>449</v>
+        <v>468</v>
       </c>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.15">
@@ -9636,10 +10220,10 @@
         <v>264</v>
       </c>
       <c r="B193" s="1">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C193" t="s">
-        <v>451</v>
+        <v>469</v>
       </c>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.15">
@@ -9647,10 +10231,10 @@
         <v>264</v>
       </c>
       <c r="B194" s="1">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C194" t="s">
-        <v>452</v>
+        <v>470</v>
       </c>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.15">
@@ -9658,10 +10242,10 @@
         <v>264</v>
       </c>
       <c r="B195" s="1">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C195" t="s">
-        <v>455</v>
+        <v>471</v>
       </c>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.15">
@@ -9669,10 +10253,10 @@
         <v>264</v>
       </c>
       <c r="B196" s="1">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C196" t="s">
-        <v>456</v>
+        <v>472</v>
       </c>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.15">
@@ -9680,10 +10264,10 @@
         <v>264</v>
       </c>
       <c r="B197" s="1">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C197" t="s">
-        <v>458</v>
+        <v>473</v>
       </c>
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.15">
@@ -9691,10 +10275,10 @@
         <v>264</v>
       </c>
       <c r="B198" s="1">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C198" t="s">
-        <v>459</v>
+        <v>474</v>
       </c>
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.15">
@@ -9702,10 +10286,10 @@
         <v>264</v>
       </c>
       <c r="B199" s="1">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C199" t="s">
-        <v>462</v>
+        <v>475</v>
       </c>
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.15">
@@ -9713,10 +10297,10 @@
         <v>264</v>
       </c>
       <c r="B200" s="1">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C200" t="s">
-        <v>463</v>
+        <v>476</v>
       </c>
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.15">
@@ -9724,10 +10308,10 @@
         <v>264</v>
       </c>
       <c r="B201" s="1">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C201" t="s">
-        <v>465</v>
+        <v>477</v>
       </c>
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.15">
@@ -9735,10 +10319,10 @@
         <v>264</v>
       </c>
       <c r="B202" s="1">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C202" t="s">
-        <v>466</v>
+        <v>478</v>
       </c>
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.15">
@@ -9746,10 +10330,10 @@
         <v>264</v>
       </c>
       <c r="B203" s="1">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C203" t="s">
-        <v>469</v>
+        <v>279</v>
       </c>
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.15">
@@ -9757,10 +10341,10 @@
         <v>264</v>
       </c>
       <c r="B204" s="1">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C204" t="s">
-        <v>470</v>
+        <v>280</v>
       </c>
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.15">
@@ -9768,10 +10352,10 @@
         <v>264</v>
       </c>
       <c r="B205" s="1">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C205" t="s">
-        <v>472</v>
+        <v>281</v>
       </c>
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.15">
@@ -9779,10 +10363,10 @@
         <v>264</v>
       </c>
       <c r="B206" s="1">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C206" t="s">
-        <v>473</v>
+        <v>282</v>
       </c>
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.15">
@@ -9790,10 +10374,10 @@
         <v>264</v>
       </c>
       <c r="B207" s="1">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C207" t="s">
-        <v>476</v>
+        <v>283</v>
       </c>
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.15">
@@ -9801,13 +10385,13 @@
         <v>264</v>
       </c>
       <c r="B208" s="1">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C208" t="s">
-        <v>477</v>
-      </c>
-    </row>
-    <row r="209" spans="1:3" x14ac:dyDescent="0.15">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="209" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A209" t="s">
         <v>264</v>
       </c>
@@ -9815,43 +10399,43 @@
         <v>34</v>
       </c>
       <c r="C209" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="210" spans="1:3" x14ac:dyDescent="0.15">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="210" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A210" t="s">
         <v>264</v>
       </c>
       <c r="B210" s="1">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C210" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="211" spans="1:3" x14ac:dyDescent="0.15">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="211" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A211" t="s">
         <v>264</v>
       </c>
       <c r="B211" s="1">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C211" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="212" spans="1:3" x14ac:dyDescent="0.15">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="212" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A212" t="s">
         <v>264</v>
       </c>
       <c r="B212" s="1">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C212" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="213" spans="1:3" x14ac:dyDescent="0.15">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="213" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A213" t="s">
         <v>264</v>
       </c>
@@ -9859,10 +10443,10 @@
         <v>35</v>
       </c>
       <c r="C213" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="214" spans="1:3" x14ac:dyDescent="0.15">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="214" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A214" t="s">
         <v>264</v>
       </c>
@@ -9870,10 +10454,10 @@
         <v>35</v>
       </c>
       <c r="C214" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="215" spans="1:3" x14ac:dyDescent="0.15">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="215" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A215" t="s">
         <v>264</v>
       </c>
@@ -9881,23 +10465,1276 @@
         <v>35</v>
       </c>
       <c r="C215" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="216" spans="1:3" x14ac:dyDescent="0.15">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="216" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A216" t="s">
-        <v>264</v>
+        <v>556</v>
       </c>
       <c r="B216" s="1">
         <v>35</v>
       </c>
       <c r="C216" t="s">
-        <v>291</v>
+        <v>558</v>
+      </c>
+    </row>
+    <row r="218" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="D218" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="219" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A219" t="s">
+        <v>557</v>
+      </c>
+      <c r="B219" s="1">
+        <v>0</v>
+      </c>
+      <c r="C219" t="s">
+        <v>608</v>
+      </c>
+      <c r="D219" t="s">
+        <v>607</v>
+      </c>
+      <c r="E219" t="s">
+        <v>494</v>
+      </c>
+      <c r="F219" t="s">
+        <v>530</v>
+      </c>
+      <c r="H219">
+        <v>12</v>
+      </c>
+      <c r="I219" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="220" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A220" t="s">
+        <v>557</v>
+      </c>
+      <c r="B220" s="1">
+        <v>1</v>
+      </c>
+      <c r="C220" t="s">
+        <v>609</v>
+      </c>
+      <c r="D220" t="s">
+        <v>583</v>
+      </c>
+      <c r="E220" t="s">
+        <v>495</v>
+      </c>
+      <c r="F220" t="s">
+        <v>531</v>
+      </c>
+      <c r="H220">
+        <v>13</v>
+      </c>
+      <c r="I220" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="221" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A221" t="s">
+        <v>557</v>
+      </c>
+      <c r="B221" s="1">
+        <v>2</v>
+      </c>
+      <c r="C221" t="s">
+        <v>610</v>
+      </c>
+      <c r="D221" t="s">
+        <v>584</v>
+      </c>
+      <c r="E221" t="s">
+        <v>496</v>
+      </c>
+      <c r="F221" t="s">
+        <v>532</v>
+      </c>
+      <c r="H221">
+        <v>14</v>
+      </c>
+      <c r="I221" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="222" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A222" t="s">
+        <v>557</v>
+      </c>
+      <c r="B222" s="1">
+        <v>3</v>
+      </c>
+      <c r="C222" t="s">
+        <v>611</v>
+      </c>
+      <c r="D222" t="s">
+        <v>585</v>
+      </c>
+      <c r="E222" t="s">
+        <v>497</v>
+      </c>
+      <c r="F222" t="s">
+        <v>533</v>
+      </c>
+      <c r="H222">
+        <v>15</v>
+      </c>
+      <c r="I222" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="223" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A223" t="s">
+        <v>557</v>
+      </c>
+      <c r="B223" s="1">
+        <v>4</v>
+      </c>
+      <c r="C223" t="s">
+        <v>612</v>
+      </c>
+      <c r="D223" t="s">
+        <v>586</v>
+      </c>
+      <c r="E223" t="s">
+        <v>498</v>
+      </c>
+      <c r="F223" t="s">
+        <v>534</v>
+      </c>
+      <c r="H223">
+        <v>16</v>
+      </c>
+      <c r="I223" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="224" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A224" t="s">
+        <v>557</v>
+      </c>
+      <c r="B224" s="1">
+        <v>5</v>
+      </c>
+      <c r="C224" t="s">
+        <v>613</v>
+      </c>
+      <c r="D224" t="s">
+        <v>587</v>
+      </c>
+      <c r="E224" t="s">
+        <v>499</v>
+      </c>
+      <c r="F224" t="s">
+        <v>535</v>
+      </c>
+      <c r="H224">
+        <v>17</v>
+      </c>
+      <c r="I224" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="225" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A225" t="s">
+        <v>557</v>
+      </c>
+      <c r="B225" s="1">
+        <v>6</v>
+      </c>
+      <c r="C225" t="s">
+        <v>614</v>
+      </c>
+      <c r="D225" t="s">
+        <v>588</v>
+      </c>
+      <c r="E225" t="s">
+        <v>500</v>
+      </c>
+      <c r="F225" t="s">
+        <v>536</v>
+      </c>
+      <c r="H225">
+        <v>18</v>
+      </c>
+      <c r="I225" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="226" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A226" t="s">
+        <v>557</v>
+      </c>
+      <c r="B226" s="1">
+        <v>7</v>
+      </c>
+      <c r="C226" t="s">
+        <v>615</v>
+      </c>
+      <c r="D226" t="s">
+        <v>589</v>
+      </c>
+      <c r="E226" t="s">
+        <v>501</v>
+      </c>
+      <c r="F226" t="s">
+        <v>537</v>
+      </c>
+      <c r="H226">
+        <v>19</v>
+      </c>
+      <c r="I226" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="227" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A227" t="s">
+        <v>557</v>
+      </c>
+      <c r="B227" s="1">
+        <v>8</v>
+      </c>
+      <c r="C227" t="s">
+        <v>616</v>
+      </c>
+      <c r="D227" t="s">
+        <v>590</v>
+      </c>
+      <c r="E227" t="s">
+        <v>502</v>
+      </c>
+      <c r="F227" t="s">
+        <v>538</v>
+      </c>
+      <c r="H227">
+        <v>20</v>
+      </c>
+      <c r="I227" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="228" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A228" t="s">
+        <v>557</v>
+      </c>
+      <c r="B228" s="1">
+        <v>9</v>
+      </c>
+      <c r="C228" t="s">
+        <v>617</v>
+      </c>
+      <c r="D228" t="s">
+        <v>591</v>
+      </c>
+      <c r="E228" t="s">
+        <v>503</v>
+      </c>
+      <c r="F228" t="s">
+        <v>539</v>
+      </c>
+      <c r="H228">
+        <v>21</v>
+      </c>
+      <c r="I228" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="229" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A229" t="s">
+        <v>557</v>
+      </c>
+      <c r="B229" s="1">
+        <v>10</v>
+      </c>
+      <c r="C229" t="s">
+        <v>618</v>
+      </c>
+      <c r="D229" t="s">
+        <v>592</v>
+      </c>
+      <c r="E229" t="s">
+        <v>504</v>
+      </c>
+      <c r="F229" t="s">
+        <v>540</v>
+      </c>
+      <c r="H229">
+        <v>22</v>
+      </c>
+      <c r="I229" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="230" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A230" t="s">
+        <v>557</v>
+      </c>
+      <c r="B230" s="1">
+        <v>11</v>
+      </c>
+      <c r="C230" t="s">
+        <v>619</v>
+      </c>
+      <c r="D230" t="s">
+        <v>593</v>
+      </c>
+      <c r="E230" t="s">
+        <v>505</v>
+      </c>
+      <c r="F230" t="s">
+        <v>541</v>
+      </c>
+      <c r="H230">
+        <v>23</v>
+      </c>
+      <c r="I230" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="232" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A232" t="s">
+        <v>557</v>
+      </c>
+      <c r="B232" s="1">
+        <v>0</v>
+      </c>
+      <c r="C232" t="s">
+        <v>620</v>
+      </c>
+      <c r="D232" t="s">
+        <v>594</v>
+      </c>
+      <c r="E232" t="s">
+        <v>494</v>
+      </c>
+      <c r="G232" t="s">
+        <v>543</v>
+      </c>
+      <c r="H232">
+        <v>12</v>
+      </c>
+      <c r="I232" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="233" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A233" t="s">
+        <v>557</v>
+      </c>
+      <c r="B233" s="1">
+        <v>1</v>
+      </c>
+      <c r="C233" t="s">
+        <v>621</v>
+      </c>
+      <c r="D233" t="s">
+        <v>595</v>
+      </c>
+      <c r="E233" t="s">
+        <v>495</v>
+      </c>
+      <c r="G233" t="s">
+        <v>545</v>
+      </c>
+      <c r="H233">
+        <v>13</v>
+      </c>
+      <c r="I233" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="234" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A234" t="s">
+        <v>557</v>
+      </c>
+      <c r="B234" s="1">
+        <v>2</v>
+      </c>
+      <c r="C234" t="s">
+        <v>622</v>
+      </c>
+      <c r="D234" t="s">
+        <v>596</v>
+      </c>
+      <c r="E234" t="s">
+        <v>496</v>
+      </c>
+      <c r="G234" t="s">
+        <v>546</v>
+      </c>
+      <c r="H234">
+        <v>14</v>
+      </c>
+      <c r="I234" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="235" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A235" t="s">
+        <v>557</v>
+      </c>
+      <c r="B235" s="1">
+        <v>3</v>
+      </c>
+      <c r="C235" t="s">
+        <v>623</v>
+      </c>
+      <c r="D235" t="s">
+        <v>597</v>
+      </c>
+      <c r="E235" t="s">
+        <v>497</v>
+      </c>
+      <c r="G235" t="s">
+        <v>547</v>
+      </c>
+      <c r="H235">
+        <v>15</v>
+      </c>
+      <c r="I235" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="236" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A236" t="s">
+        <v>557</v>
+      </c>
+      <c r="B236" s="1">
+        <v>4</v>
+      </c>
+      <c r="C236" t="s">
+        <v>624</v>
+      </c>
+      <c r="D236" t="s">
+        <v>598</v>
+      </c>
+      <c r="E236" t="s">
+        <v>498</v>
+      </c>
+      <c r="G236" t="s">
+        <v>548</v>
+      </c>
+      <c r="H236">
+        <v>16</v>
+      </c>
+      <c r="I236" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="237" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A237" t="s">
+        <v>557</v>
+      </c>
+      <c r="B237" s="1">
+        <v>5</v>
+      </c>
+      <c r="C237" t="s">
+        <v>625</v>
+      </c>
+      <c r="D237" t="s">
+        <v>599</v>
+      </c>
+      <c r="E237" t="s">
+        <v>499</v>
+      </c>
+      <c r="G237" t="s">
+        <v>549</v>
+      </c>
+      <c r="H237">
+        <v>17</v>
+      </c>
+      <c r="I237" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="238" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A238" t="s">
+        <v>557</v>
+      </c>
+      <c r="B238" s="1">
+        <v>6</v>
+      </c>
+      <c r="C238" t="s">
+        <v>626</v>
+      </c>
+      <c r="D238" t="s">
+        <v>600</v>
+      </c>
+      <c r="E238" t="s">
+        <v>500</v>
+      </c>
+      <c r="G238" t="s">
+        <v>550</v>
+      </c>
+      <c r="H238">
+        <v>18</v>
+      </c>
+      <c r="I238" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="239" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A239" t="s">
+        <v>557</v>
+      </c>
+      <c r="B239" s="1">
+        <v>7</v>
+      </c>
+      <c r="C239" t="s">
+        <v>627</v>
+      </c>
+      <c r="D239" t="s">
+        <v>601</v>
+      </c>
+      <c r="E239" t="s">
+        <v>501</v>
+      </c>
+      <c r="G239" t="s">
+        <v>551</v>
+      </c>
+      <c r="H239">
+        <v>19</v>
+      </c>
+      <c r="I239" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="240" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A240" t="s">
+        <v>557</v>
+      </c>
+      <c r="B240" s="1">
+        <v>8</v>
+      </c>
+      <c r="C240" t="s">
+        <v>628</v>
+      </c>
+      <c r="D240" t="s">
+        <v>602</v>
+      </c>
+      <c r="E240" t="s">
+        <v>502</v>
+      </c>
+      <c r="G240" t="s">
+        <v>552</v>
+      </c>
+      <c r="H240">
+        <v>20</v>
+      </c>
+      <c r="I240" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="241" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A241" t="s">
+        <v>557</v>
+      </c>
+      <c r="B241" s="1">
+        <v>9</v>
+      </c>
+      <c r="C241" t="s">
+        <v>629</v>
+      </c>
+      <c r="D241" t="s">
+        <v>603</v>
+      </c>
+      <c r="E241" t="s">
+        <v>503</v>
+      </c>
+      <c r="G241" t="s">
+        <v>553</v>
+      </c>
+      <c r="H241">
+        <v>21</v>
+      </c>
+      <c r="I241" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="242" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A242" t="s">
+        <v>557</v>
+      </c>
+      <c r="B242" s="1">
+        <v>10</v>
+      </c>
+      <c r="C242" t="s">
+        <v>630</v>
+      </c>
+      <c r="D242" t="s">
+        <v>604</v>
+      </c>
+      <c r="E242" t="s">
+        <v>504</v>
+      </c>
+      <c r="G242" t="s">
+        <v>554</v>
+      </c>
+      <c r="H242">
+        <v>22</v>
+      </c>
+      <c r="I242" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="243" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A243" t="s">
+        <v>557</v>
+      </c>
+      <c r="B243" s="1">
+        <v>11</v>
+      </c>
+      <c r="C243" t="s">
+        <v>631</v>
+      </c>
+      <c r="D243" t="s">
+        <v>605</v>
+      </c>
+      <c r="E243" t="s">
+        <v>505</v>
+      </c>
+      <c r="G243" t="s">
+        <v>555</v>
+      </c>
+      <c r="H243">
+        <v>23</v>
+      </c>
+      <c r="I243" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="246" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A246" t="s">
+        <v>557</v>
+      </c>
+      <c r="B246" s="1">
+        <v>12</v>
+      </c>
+      <c r="C246" t="s">
+        <v>632</v>
+      </c>
+      <c r="D246" t="s">
+        <v>530</v>
+      </c>
+      <c r="E246" t="s">
+        <v>518</v>
+      </c>
+      <c r="F246" t="s">
+        <v>559</v>
+      </c>
+      <c r="H246">
+        <v>24</v>
+      </c>
+      <c r="I246" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="247" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A247" t="s">
+        <v>557</v>
+      </c>
+      <c r="B247" s="1">
+        <v>13</v>
+      </c>
+      <c r="C247" t="s">
+        <v>633</v>
+      </c>
+      <c r="D247" t="s">
+        <v>531</v>
+      </c>
+      <c r="E247" t="s">
+        <v>519</v>
+      </c>
+      <c r="F247" t="s">
+        <v>560</v>
+      </c>
+      <c r="H247">
+        <v>25</v>
+      </c>
+      <c r="I247" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="248" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A248" t="s">
+        <v>557</v>
+      </c>
+      <c r="B248" s="1">
+        <v>14</v>
+      </c>
+      <c r="C248" t="s">
+        <v>634</v>
+      </c>
+      <c r="D248" t="s">
+        <v>532</v>
+      </c>
+      <c r="E248" t="s">
+        <v>520</v>
+      </c>
+      <c r="F248" t="s">
+        <v>561</v>
+      </c>
+      <c r="H248">
+        <v>26</v>
+      </c>
+      <c r="I248" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="249" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A249" t="s">
+        <v>557</v>
+      </c>
+      <c r="B249" s="1">
+        <v>15</v>
+      </c>
+      <c r="C249" t="s">
+        <v>635</v>
+      </c>
+      <c r="D249" t="s">
+        <v>533</v>
+      </c>
+      <c r="E249" t="s">
+        <v>521</v>
+      </c>
+      <c r="F249" t="s">
+        <v>562</v>
+      </c>
+      <c r="H249">
+        <v>27</v>
+      </c>
+      <c r="I249" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="250" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A250" t="s">
+        <v>557</v>
+      </c>
+      <c r="B250" s="1">
+        <v>16</v>
+      </c>
+      <c r="C250" t="s">
+        <v>636</v>
+      </c>
+      <c r="D250" t="s">
+        <v>534</v>
+      </c>
+      <c r="E250" t="s">
+        <v>522</v>
+      </c>
+      <c r="F250" t="s">
+        <v>563</v>
+      </c>
+      <c r="H250">
+        <v>28</v>
+      </c>
+      <c r="I250" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="251" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A251" t="s">
+        <v>557</v>
+      </c>
+      <c r="B251" s="1">
+        <v>17</v>
+      </c>
+      <c r="C251" t="s">
+        <v>637</v>
+      </c>
+      <c r="D251" t="s">
+        <v>535</v>
+      </c>
+      <c r="E251" t="s">
+        <v>523</v>
+      </c>
+      <c r="F251" t="s">
+        <v>606</v>
+      </c>
+      <c r="H251">
+        <v>29</v>
+      </c>
+      <c r="I251" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="252" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A252" t="s">
+        <v>557</v>
+      </c>
+      <c r="B252" s="1">
+        <v>18</v>
+      </c>
+      <c r="C252" t="s">
+        <v>638</v>
+      </c>
+      <c r="D252" t="s">
+        <v>536</v>
+      </c>
+      <c r="E252" t="s">
+        <v>524</v>
+      </c>
+      <c r="F252" t="s">
+        <v>564</v>
+      </c>
+      <c r="H252">
+        <v>30</v>
+      </c>
+      <c r="I252" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="253" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A253" t="s">
+        <v>557</v>
+      </c>
+      <c r="B253" s="1">
+        <v>19</v>
+      </c>
+      <c r="C253" t="s">
+        <v>639</v>
+      </c>
+      <c r="D253" t="s">
+        <v>537</v>
+      </c>
+      <c r="E253" t="s">
+        <v>525</v>
+      </c>
+      <c r="F253" t="s">
+        <v>565</v>
+      </c>
+      <c r="H253">
+        <v>31</v>
+      </c>
+      <c r="I253" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="254" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A254" t="s">
+        <v>557</v>
+      </c>
+      <c r="B254" s="1">
+        <v>20</v>
+      </c>
+      <c r="C254" t="s">
+        <v>640</v>
+      </c>
+      <c r="D254" t="s">
+        <v>538</v>
+      </c>
+      <c r="E254" t="s">
+        <v>526</v>
+      </c>
+      <c r="F254" t="s">
+        <v>566</v>
+      </c>
+      <c r="H254">
+        <v>32</v>
+      </c>
+      <c r="I254" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="255" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A255" t="s">
+        <v>557</v>
+      </c>
+      <c r="B255" s="1">
+        <v>21</v>
+      </c>
+      <c r="C255" t="s">
+        <v>641</v>
+      </c>
+      <c r="D255" t="s">
+        <v>539</v>
+      </c>
+      <c r="E255" t="s">
+        <v>527</v>
+      </c>
+      <c r="F255" t="s">
+        <v>567</v>
+      </c>
+      <c r="H255">
+        <v>33</v>
+      </c>
+      <c r="I255" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="256" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A256" t="s">
+        <v>557</v>
+      </c>
+      <c r="B256" s="1">
+        <v>22</v>
+      </c>
+      <c r="C256" t="s">
+        <v>642</v>
+      </c>
+      <c r="D256" t="s">
+        <v>540</v>
+      </c>
+      <c r="E256" t="s">
+        <v>528</v>
+      </c>
+      <c r="F256" t="s">
+        <v>568</v>
+      </c>
+      <c r="H256">
+        <v>34</v>
+      </c>
+      <c r="I256" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="257" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A257" t="s">
+        <v>557</v>
+      </c>
+      <c r="B257" s="1">
+        <v>23</v>
+      </c>
+      <c r="C257" t="s">
+        <v>643</v>
+      </c>
+      <c r="D257" t="s">
+        <v>541</v>
+      </c>
+      <c r="E257" t="s">
+        <v>529</v>
+      </c>
+      <c r="F257" t="s">
+        <v>569</v>
+      </c>
+      <c r="H257">
+        <v>35</v>
+      </c>
+      <c r="I257" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="259" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A259" t="s">
+        <v>557</v>
+      </c>
+      <c r="B259" s="1">
+        <v>12</v>
+      </c>
+      <c r="C259" t="s">
+        <v>644</v>
+      </c>
+      <c r="D259" t="s">
+        <v>542</v>
+      </c>
+      <c r="E259" t="s">
+        <v>518</v>
+      </c>
+      <c r="G259" t="s">
+        <v>570</v>
+      </c>
+      <c r="H259">
+        <v>24</v>
+      </c>
+      <c r="I259" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="260" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A260" t="s">
+        <v>557</v>
+      </c>
+      <c r="B260" s="1">
+        <v>13</v>
+      </c>
+      <c r="C260" t="s">
+        <v>645</v>
+      </c>
+      <c r="D260" t="s">
+        <v>544</v>
+      </c>
+      <c r="E260" t="s">
+        <v>519</v>
+      </c>
+      <c r="G260" t="s">
+        <v>571</v>
+      </c>
+      <c r="H260">
+        <v>25</v>
+      </c>
+      <c r="I260" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="261" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A261" t="s">
+        <v>557</v>
+      </c>
+      <c r="B261" s="1">
+        <v>14</v>
+      </c>
+      <c r="C261" t="s">
+        <v>646</v>
+      </c>
+      <c r="D261" t="s">
+        <v>546</v>
+      </c>
+      <c r="E261" t="s">
+        <v>520</v>
+      </c>
+      <c r="G261" t="s">
+        <v>572</v>
+      </c>
+      <c r="H261">
+        <v>26</v>
+      </c>
+      <c r="I261" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="262" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A262" t="s">
+        <v>557</v>
+      </c>
+      <c r="B262" s="1">
+        <v>15</v>
+      </c>
+      <c r="C262" t="s">
+        <v>647</v>
+      </c>
+      <c r="D262" t="s">
+        <v>547</v>
+      </c>
+      <c r="E262" t="s">
+        <v>521</v>
+      </c>
+      <c r="G262" t="s">
+        <v>573</v>
+      </c>
+      <c r="H262">
+        <v>27</v>
+      </c>
+      <c r="I262" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="263" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A263" t="s">
+        <v>557</v>
+      </c>
+      <c r="B263" s="1">
+        <v>16</v>
+      </c>
+      <c r="C263" t="s">
+        <v>648</v>
+      </c>
+      <c r="D263" t="s">
+        <v>548</v>
+      </c>
+      <c r="E263" t="s">
+        <v>522</v>
+      </c>
+      <c r="G263" t="s">
+        <v>574</v>
+      </c>
+      <c r="H263">
+        <v>28</v>
+      </c>
+      <c r="I263" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="264" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A264" t="s">
+        <v>557</v>
+      </c>
+      <c r="B264" s="1">
+        <v>17</v>
+      </c>
+      <c r="C264" t="s">
+        <v>649</v>
+      </c>
+      <c r="D264" t="s">
+        <v>549</v>
+      </c>
+      <c r="E264" t="s">
+        <v>523</v>
+      </c>
+      <c r="G264" t="s">
+        <v>575</v>
+      </c>
+      <c r="H264">
+        <v>29</v>
+      </c>
+      <c r="I264" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="265" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A265" t="s">
+        <v>557</v>
+      </c>
+      <c r="B265" s="1">
+        <v>18</v>
+      </c>
+      <c r="C265" t="s">
+        <v>650</v>
+      </c>
+      <c r="D265" t="s">
+        <v>550</v>
+      </c>
+      <c r="E265" t="s">
+        <v>524</v>
+      </c>
+      <c r="G265" t="s">
+        <v>576</v>
+      </c>
+      <c r="H265">
+        <v>30</v>
+      </c>
+      <c r="I265" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="266" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A266" t="s">
+        <v>557</v>
+      </c>
+      <c r="B266" s="1">
+        <v>19</v>
+      </c>
+      <c r="C266" t="s">
+        <v>651</v>
+      </c>
+      <c r="D266" t="s">
+        <v>551</v>
+      </c>
+      <c r="E266" t="s">
+        <v>525</v>
+      </c>
+      <c r="G266" t="s">
+        <v>577</v>
+      </c>
+      <c r="H266">
+        <v>31</v>
+      </c>
+      <c r="I266" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="267" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A267" t="s">
+        <v>557</v>
+      </c>
+      <c r="B267" s="1">
+        <v>20</v>
+      </c>
+      <c r="C267" t="s">
+        <v>652</v>
+      </c>
+      <c r="D267" t="s">
+        <v>552</v>
+      </c>
+      <c r="E267" t="s">
+        <v>526</v>
+      </c>
+      <c r="G267" t="s">
+        <v>578</v>
+      </c>
+      <c r="H267">
+        <v>32</v>
+      </c>
+      <c r="I267" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="268" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A268" t="s">
+        <v>557</v>
+      </c>
+      <c r="B268" s="1">
+        <v>21</v>
+      </c>
+      <c r="C268" t="s">
+        <v>653</v>
+      </c>
+      <c r="D268" t="s">
+        <v>553</v>
+      </c>
+      <c r="E268" t="s">
+        <v>527</v>
+      </c>
+      <c r="G268" t="s">
+        <v>579</v>
+      </c>
+      <c r="H268">
+        <v>33</v>
+      </c>
+      <c r="I268" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="269" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A269" t="s">
+        <v>557</v>
+      </c>
+      <c r="B269" s="1">
+        <v>22</v>
+      </c>
+      <c r="C269" t="s">
+        <v>654</v>
+      </c>
+      <c r="D269" t="s">
+        <v>554</v>
+      </c>
+      <c r="E269" t="s">
+        <v>528</v>
+      </c>
+      <c r="G269" t="s">
+        <v>580</v>
+      </c>
+      <c r="H269">
+        <v>34</v>
+      </c>
+      <c r="I269" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="270" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A270" t="s">
+        <v>557</v>
+      </c>
+      <c r="B270" s="1">
+        <v>23</v>
+      </c>
+      <c r="C270" t="s">
+        <v>655</v>
+      </c>
+      <c r="D270" t="s">
+        <v>555</v>
+      </c>
+      <c r="E270" t="s">
+        <v>529</v>
+      </c>
+      <c r="G270" t="s">
+        <v>581</v>
+      </c>
+      <c r="H270">
+        <v>35</v>
+      </c>
+      <c r="I270" t="s">
+        <v>517</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A1:C216">
-    <sortCondition ref="B1:B216"/>
+  <sortState ref="A1:C265">
+    <sortCondition ref="B1:B265"/>
   </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>